<commit_message>
Read fab port scenarios from port-scenarios not generic_facilities
</commit_message>
<xml_diff>
--- a/fabrication_ports/ports_scenario.xlsx
+++ b/fabrication_ports/ports_scenario.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mshields\Documents\Projects\Supply Chain Roadmap\Analysis repos\Roadmap\fabrication_ports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{265A7C0C-60C9-4157-B4C5-08E9730DB5D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9542B7D-1294-497C-93AE-1F5B71D1B7DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Scenario" sheetId="9" r:id="rId1"/>
+    <sheet name="Avg Demand Scenario" sheetId="9" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId2"/>
+    <pivotCache cacheId="2" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -565,7 +565,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Scenario!$F$8</c:f>
+              <c:f>'Avg Demand Scenario'!$F$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -584,7 +584,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Scenario!$B$9:$B$33</c:f>
+              <c:f>'Avg Demand Scenario'!$B$9:$B$33</c:f>
               <c:strCache>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
@@ -667,7 +667,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Scenario!$F$9:$F$33</c:f>
+              <c:f>'Avg Demand Scenario'!$F$9:$F$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -760,7 +760,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Scenario!$K$8</c:f>
+              <c:f>'Avg Demand Scenario'!$K$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -781,7 +781,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Scenario!$B$9:$B$33</c:f>
+              <c:f>'Avg Demand Scenario'!$B$9:$B$33</c:f>
               <c:strCache>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
@@ -864,7 +864,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Scenario!$K$9:$K$33</c:f>
+              <c:f>'Avg Demand Scenario'!$K$9:$K$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -1170,7 +1170,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[filtered_component_ports_scenario.xlsx]Scenario!PivotTable5</c:name>
+    <c:name>[ports_scenario.xlsx]Avg Demand Scenario!PivotTable5</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -1299,7 +1299,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Scenario!$H$37</c:f>
+              <c:f>'Avg Demand Scenario'!$H$37</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1320,7 +1320,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Scenario!$G$38:$G$50</c:f>
+              <c:f>'Avg Demand Scenario'!$G$38:$G$50</c:f>
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
@@ -1364,7 +1364,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Scenario!$H$38:$H$50</c:f>
+              <c:f>'Avg Demand Scenario'!$H$38:$H$50</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -2800,7 +2800,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Shields, Matt" refreshedDate="44741.711112847224" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="24" xr:uid="{0F69996E-E092-4D5B-8AF6-02BA8AF1D466}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A8:K33" sheet="Scenario"/>
+    <worksheetSource ref="A8:K33" sheet="Avg Demand Scenario"/>
   </cacheSource>
   <cacheFields count="11">
     <cacheField name="Component" numFmtId="0">
@@ -3201,7 +3201,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{391C8580-0FAE-4DE9-AE5F-736ACC565C2E}" name="PivotTable5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{391C8580-0FAE-4DE9-AE5F-736ACC565C2E}" name="PivotTable5" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="G37:H50" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField showAll="0"/>
@@ -3620,8 +3620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F1FF48-4396-4FE3-ABD9-234FB66F60F4}">
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added WC scenarios.  Added flanges and castings
</commit_message>
<xml_diff>
--- a/fabrication_ports/ports_scenario.xlsx
+++ b/fabrication_ports/ports_scenario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mshields\Documents\Projects\Supply Chain Roadmap\Analysis repos\Roadmap\fabrication_ports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9542B7D-1294-497C-93AE-1F5B71D1B7DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD9F57B-1AA3-4966-8420-9368CD77A6AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId2"/>
+    <pivotCache cacheId="17" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="139">
   <si>
     <t>Port</t>
   </si>
@@ -253,9 +253,6 @@
     <t>Smulders</t>
   </si>
   <si>
-    <t>TP 1</t>
-  </si>
-  <si>
     <t>Port of Coeymans</t>
   </si>
   <si>
@@ -368,13 +365,100 @@
   </si>
   <si>
     <t>Minimal port upgrades needed.  Need wet sotrage space.  Later announcement date due to lower TRL of GBF</t>
+  </si>
+  <si>
+    <t>Transition piece 1</t>
+  </si>
+  <si>
+    <t>Casting</t>
+  </si>
+  <si>
+    <t>Casting 1</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doesn't need to be at a port.  Exising large foundries in OH, PA. </t>
+  </si>
+  <si>
+    <t>Semisubmersible</t>
+  </si>
+  <si>
+    <t>Semisubmersible 1</t>
+  </si>
+  <si>
+    <t>Semisubmersible 2</t>
+  </si>
+  <si>
+    <t>Semisubmersible 3</t>
+  </si>
+  <si>
+    <t>Stationkeeping</t>
+  </si>
+  <si>
+    <t>Mooring chain 1</t>
+  </si>
+  <si>
+    <t>Mooring rope 1</t>
+  </si>
+  <si>
+    <t>Blade 4</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>Nacelle 2</t>
+  </si>
+  <si>
+    <t>Tower 3</t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>West Coast</t>
+  </si>
+  <si>
+    <t>TBD - Humboldt</t>
+  </si>
+  <si>
+    <t>TBD - Central Coast</t>
+  </si>
+  <si>
+    <t>TBD - Coos Bay</t>
+  </si>
+  <si>
+    <t>TBD - WA</t>
+  </si>
+  <si>
+    <t>WA</t>
+  </si>
+  <si>
+    <t>Assume fabricaiton elsewhere (GOM, Asia) and assembly at marshalling site.  Somewhat industrialized.  Don't need major facility upgrades (beyond port fab)</t>
+  </si>
+  <si>
+    <t>Flange</t>
+  </si>
+  <si>
+    <t>Flange 1</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>Schiller Newington, Portsmouth</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -394,6 +478,12 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -584,9 +674,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Avg Demand Scenario'!$B$9:$B$33</c:f>
+              <c:f>'Avg Demand Scenario'!$B$9:$B$36</c:f>
               <c:strCache>
-                <c:ptCount val="25"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>SGRE</c:v>
                 </c:pt>
@@ -600,66 +690,75 @@
                   <c:v>Blade 3</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>Blade 4</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>GE</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>Vestas</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>Nacelle 1</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
+                  <c:v>Nacelle 2</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>Marmen Welcon</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>Tower 1</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>Tower 2</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
+                  <c:v>Tower 3</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>EEW</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>US Wind</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="15">
                   <c:v>Jacket 1</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="16">
                   <c:v>GBF 1</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="17">
                   <c:v>Smulders</c:v>
                 </c:pt>
-                <c:pt idx="15">
-                  <c:v>TP 1</c:v>
-                </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="18">
+                  <c:v>Transition piece 1</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>Hellenic</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="20">
                   <c:v>Array cable 1</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="21">
                   <c:v>Array cable 2</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="22">
                   <c:v>Nexans</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="23">
                   <c:v>Prysmian</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="24">
                   <c:v>Export cable 1</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="25">
                   <c:v>Export cable 2</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="26">
                   <c:v>Nucor</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="27">
                   <c:v>Steel plate 1</c:v>
                 </c:pt>
               </c:strCache>
@@ -667,10 +766,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Avg Demand Scenario'!$F$9:$F$33</c:f>
+              <c:f>'Avg Demand Scenario'!$F$9:$F$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>2021</c:v>
                 </c:pt>
@@ -684,34 +783,34 @@
                   <c:v>2023</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2021</c:v>
+                  <c:v>2024</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>2021</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>2023</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2021</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>2023</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>2023</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>2020</c:v>
-                </c:pt>
                 <c:pt idx="11">
-                  <c:v>2021</c:v>
+                  <c:v>2023</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>2023</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2025</c:v>
+                  <c:v>2020</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>2021</c:v>
@@ -720,30 +819,39 @@
                   <c:v>2023</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>2021</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>2023</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>2023</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2018</c:v>
+                  <c:v>2021</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2021</c:v>
+                  <c:v>2023</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>2023</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2023</c:v>
+                  <c:v>2018</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>2021</c:v>
                 </c:pt>
                 <c:pt idx="24">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="27">
                   <c:v>2023</c:v>
                 </c:pt>
               </c:numCache>
@@ -781,9 +889,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Avg Demand Scenario'!$B$9:$B$33</c:f>
+              <c:f>'Avg Demand Scenario'!$B$9:$B$36</c:f>
               <c:strCache>
-                <c:ptCount val="25"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>SGRE</c:v>
                 </c:pt>
@@ -797,66 +905,75 @@
                   <c:v>Blade 3</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>Blade 4</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>GE</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>Vestas</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>Nacelle 1</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
+                  <c:v>Nacelle 2</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>Marmen Welcon</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>Tower 1</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>Tower 2</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
+                  <c:v>Tower 3</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>EEW</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>US Wind</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="15">
                   <c:v>Jacket 1</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="16">
                   <c:v>GBF 1</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="17">
                   <c:v>Smulders</c:v>
                 </c:pt>
-                <c:pt idx="15">
-                  <c:v>TP 1</c:v>
-                </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="18">
+                  <c:v>Transition piece 1</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>Hellenic</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="20">
                   <c:v>Array cable 1</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="21">
                   <c:v>Array cable 2</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="22">
                   <c:v>Nexans</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="23">
                   <c:v>Prysmian</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="24">
                   <c:v>Export cable 1</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="25">
                   <c:v>Export cable 2</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="26">
                   <c:v>Nucor</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="27">
                   <c:v>Steel plate 1</c:v>
                 </c:pt>
               </c:strCache>
@@ -864,10 +981,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Avg Demand Scenario'!$K$9:$K$33</c:f>
+              <c:f>'Avg Demand Scenario'!$K$9:$K$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -881,7 +998,7 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>5</c:v>
@@ -890,43 +1007,43 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="16">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="17">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="18">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="19">
                   <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>6</c:v>
@@ -935,12 +1052,21 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="22">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="23">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="26">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="27">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -1170,36 +1296,11 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[ports_scenario.xlsx]Avg Demand Scenario!PivotTable5</c:name>
-    <c:fmtId val="0"/>
+    <c:name>[ports_scenario.xlsx]Avg Demand Scenario!PivotTable1</c:name>
+    <c:fmtId val="1"/>
   </c:pivotSource>
   <c:chart>
     <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Number of facilities per state</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1299,7 +1400,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Avg Demand Scenario'!$H$37</c:f>
+              <c:f>'Avg Demand Scenario'!$H$48</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1320,56 +1421,71 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Avg Demand Scenario'!$G$38:$G$50</c:f>
+              <c:f>'Avg Demand Scenario'!$G$49:$G$66</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
+                  <c:v>CA</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>GA</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>KY</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>LA</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>MA</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>MD</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>ME</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>NC</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
+                  <c:v>NH</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>NJ</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>NY</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
+                  <c:v>OR</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>PA</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>RI</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="14">
                   <c:v>SC</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="15">
                   <c:v>VA</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>WA</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Avg Demand Scenario'!$H$38:$H$50</c:f>
+              <c:f>'Avg Demand Scenario'!$H$49:$H$66</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
@@ -1378,30 +1494,45 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
@@ -1409,7 +1540,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-03F9-4D8A-8A75-41ECCB557DAB}"/>
+              <c16:uniqueId val="{00000000-F9C3-45AA-AF84-5B194108A867}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1423,11 +1554,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="845487984"/>
-        <c:axId val="845492576"/>
+        <c:axId val="854290856"/>
+        <c:axId val="854290200"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="845487984"/>
+        <c:axId val="854290856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1470,7 +1601,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="845492576"/>
+        <c:crossAx val="854290200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1478,7 +1609,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="845492576"/>
+        <c:axId val="854290200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1529,7 +1660,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="845487984"/>
+        <c:crossAx val="854290856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2726,13 +2857,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>30254</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>58177</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>209736</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>77</xdr:row>
       <xdr:rowOff>75266</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2761,22 +2892,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>274543</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>45943</xdr:rowOff>
+      <xdr:colOff>898921</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>75008</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1689659</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>96556</xdr:rowOff>
+      <xdr:colOff>2458640</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>151208</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D21E5900-5CD5-97F3-8ABC-20DA520747DF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62FBFC76-7600-834B-A19C-082FC73E5751}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2798,31 +2929,35 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Shields, Matt" refreshedDate="44741.711112847224" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="24" xr:uid="{0F69996E-E092-4D5B-8AF6-02BA8AF1D466}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Shields, Matt" refreshedDate="44770.98404166667" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="35" xr:uid="{8520C2B9-52CF-46B0-8F6A-64DE6645DC34}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A8:K33" sheet="Avg Demand Scenario"/>
+    <worksheetSource ref="A8:K43" sheet="Avg Demand Scenario"/>
   </cacheSource>
   <cacheFields count="11">
     <cacheField name="Component" numFmtId="0">
       <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="Factory" numFmtId="0">
-      <sharedItems count="24">
+      <sharedItems count="35">
         <s v="SGRE"/>
         <s v="Blade 1"/>
         <s v="Blade 2"/>
         <s v="Blade 3"/>
+        <s v="Blade 4"/>
         <s v="GE"/>
         <s v="Vestas"/>
         <s v="Nacelle 1"/>
+        <s v="Nacelle 2"/>
         <s v="Marmen Welcon"/>
         <s v="Tower 1"/>
         <s v="Tower 2"/>
+        <s v="Tower 3"/>
         <s v="EEW"/>
         <s v="US Wind"/>
         <s v="Jacket 1"/>
+        <s v="GBF 1"/>
         <s v="Smulders"/>
-        <s v="TP 1"/>
+        <s v="Transition piece 1"/>
         <s v="Hellenic"/>
         <s v="Array cable 1"/>
         <s v="Array cable 2"/>
@@ -2832,17 +2967,53 @@
         <s v="Export cable 2"/>
         <s v="Nucor"/>
         <s v="Steel plate 1"/>
+        <s v="Casting 1"/>
+        <s v="Flange 1"/>
+        <s v="Semisubmersible 1"/>
+        <s v="Semisubmersible 2"/>
+        <s v="Semisubmersible 3"/>
+        <s v="Mooring chain 1"/>
+        <s v="Mooring rope 1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Port" numFmtId="0">
-      <sharedItems/>
+      <sharedItems containsBlank="1" count="26">
+        <s v="Portsmouth Marine Terminal"/>
+        <s v="General Cargo Terminal at Port of Wilmington"/>
+        <s v="Newport News Marine Terminal"/>
+        <s v="New Jersey Wind Port"/>
+        <s v="TBD - Coos Bay"/>
+        <s v="South Quay"/>
+        <s v="TBD - Humboldt"/>
+        <s v="Port of Albany"/>
+        <s v="Tradepoint Atlantic"/>
+        <s v="Searsport"/>
+        <s v="Port of Paulsboro"/>
+        <s v="Port of New Orleans"/>
+        <s v="Radio Island, Morehead City"/>
+        <s v="Port of Coeymans"/>
+        <s v="Arthur Kill Terminal"/>
+        <s v="Mystic River, Everett"/>
+        <s v="Goose Island"/>
+        <s v="Brayton Point"/>
+        <s v="Quonset Business Park / Port of Davisville"/>
+        <s v="Columbus Terminal"/>
+        <s v="Brandenburg "/>
+        <s v="Port of Brunswick"/>
+        <m/>
+        <s v="Schiller Newington, Portsmouth"/>
+        <s v="TBD - Central Coast"/>
+        <s v="TBD - WA"/>
+      </sharedItems>
     </cacheField>
     <cacheField name="State" numFmtId="0">
-      <sharedItems count="12">
+      <sharedItems count="17">
         <s v="VA"/>
         <s v="NC"/>
         <s v="NJ"/>
+        <s v="OR"/>
         <s v="RI"/>
+        <s v="CA"/>
         <s v="NY"/>
         <s v="MD"/>
         <s v="ME"/>
@@ -2851,28 +3022,31 @@
         <s v="SC"/>
         <s v="KY"/>
         <s v="GA"/>
+        <s v="PA"/>
+        <s v="NH"/>
+        <s v="WA"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Region" numFmtId="0">
       <sharedItems/>
     </cacheField>
     <cacheField name="Announcement date" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2018" maxValue="2023"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2018" maxValue="2026"/>
     </cacheField>
     <cacheField name="Port upgrade duration (yrs)" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="3" maxValue="3"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="4"/>
     </cacheField>
     <cacheField name="Facility construction (yrs)" numFmtId="0">
       <sharedItems containsMixedTypes="1" containsNumber="1" minValue="1" maxValue="5"/>
     </cacheField>
     <cacheField name="Port/facility overlap (%)" numFmtId="0">
-      <sharedItems containsMixedTypes="1" containsNumber="1" minValue="0.2" maxValue="0.8"/>
+      <sharedItems containsMixedTypes="1" containsNumber="1" minValue="0" maxValue="0.8"/>
     </cacheField>
     <cacheField name="Operational date" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2020" maxValue="2030"/>
     </cacheField>
     <cacheField name="Duration" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2" maxValue="7"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2" maxValue="6"/>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -2884,11 +3058,11 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="24">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="35">
   <r>
     <s v="Blade"/>
     <x v="0"/>
-    <s v="Portsmouth Marine Terminal"/>
+    <x v="0"/>
     <x v="0"/>
     <s v="South Atlantic"/>
     <n v="2021"/>
@@ -2901,7 +3075,7 @@
   <r>
     <m/>
     <x v="1"/>
-    <s v="General Cargo Terminal at Port of Wilmington"/>
+    <x v="1"/>
     <x v="1"/>
     <s v="South Atlantic"/>
     <n v="2023"/>
@@ -2914,7 +3088,7 @@
   <r>
     <m/>
     <x v="2"/>
-    <s v="Newport News Marine Terminal"/>
+    <x v="2"/>
     <x v="0"/>
     <s v="South Atlantic"/>
     <n v="2023"/>
@@ -2927,7 +3101,7 @@
   <r>
     <m/>
     <x v="3"/>
-    <s v="New Jersey Wind Port"/>
+    <x v="3"/>
     <x v="2"/>
     <s v="Central Atlantic"/>
     <n v="2023"/>
@@ -2938,22 +3112,22 @@
     <n v="5"/>
   </r>
   <r>
-    <s v="Nacelle"/>
+    <m/>
     <x v="4"/>
-    <s v="New Jersey Wind Port"/>
-    <x v="2"/>
-    <s v="Central Atlantic"/>
-    <n v="2021"/>
+    <x v="4"/>
+    <x v="3"/>
+    <s v="West Coast"/>
+    <n v="2024"/>
+    <n v="4"/>
     <n v="3"/>
-    <n v="3"/>
-    <n v="0.33333333333333331"/>
-    <n v="2026"/>
-    <n v="5"/>
+    <n v="0.25"/>
+    <n v="2030"/>
+    <n v="6"/>
   </r>
   <r>
-    <m/>
+    <s v="Nacelle"/>
     <x v="5"/>
-    <s v="New Jersey Wind Port"/>
+    <x v="3"/>
     <x v="2"/>
     <s v="Central Atlantic"/>
     <n v="2021"/>
@@ -2966,8 +3140,21 @@
   <r>
     <m/>
     <x v="6"/>
-    <s v="South Quay"/>
     <x v="3"/>
+    <x v="2"/>
+    <s v="Central Atlantic"/>
+    <n v="2021"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="0.33333333333333331"/>
+    <n v="2026"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <m/>
+    <x v="7"/>
+    <x v="5"/>
+    <x v="4"/>
     <s v="North Atlantic"/>
     <n v="2023"/>
     <n v="3"/>
@@ -2977,10 +3164,23 @@
     <n v="5"/>
   </r>
   <r>
+    <m/>
+    <x v="8"/>
+    <x v="6"/>
+    <x v="5"/>
+    <s v="West Coast"/>
+    <n v="2023"/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="0.25"/>
+    <n v="2029"/>
+    <n v="6"/>
+  </r>
+  <r>
     <s v="Tower"/>
+    <x v="9"/>
     <x v="7"/>
-    <s v="Port of Albany"/>
-    <x v="4"/>
+    <x v="6"/>
     <s v="Central Atlantic"/>
     <n v="2021"/>
     <n v="3"/>
@@ -2991,9 +3191,9 @@
   </r>
   <r>
     <m/>
+    <x v="10"/>
     <x v="8"/>
-    <s v="Tradepoint Atlantic"/>
-    <x v="5"/>
+    <x v="7"/>
     <s v="South Atlantic"/>
     <n v="2023"/>
     <n v="3"/>
@@ -3004,9 +3204,9 @@
   </r>
   <r>
     <m/>
+    <x v="11"/>
     <x v="9"/>
-    <s v="Searsport"/>
-    <x v="6"/>
+    <x v="8"/>
     <s v="North Atlantic"/>
     <n v="2023"/>
     <n v="3"/>
@@ -3016,9 +3216,22 @@
     <n v="4"/>
   </r>
   <r>
+    <m/>
+    <x v="12"/>
+    <x v="6"/>
+    <x v="5"/>
+    <s v="West Coast"/>
+    <n v="2023"/>
+    <n v="4"/>
+    <n v="2.5"/>
+    <n v="0.25"/>
+    <n v="2028"/>
+    <n v="5"/>
+  </r>
+  <r>
     <s v="Monopile"/>
+    <x v="13"/>
     <x v="10"/>
-    <s v="Port of Paulsboro"/>
     <x v="2"/>
     <s v="Central Atlantic"/>
     <n v="2020"/>
@@ -3030,8 +3243,8 @@
   </r>
   <r>
     <m/>
-    <x v="11"/>
-    <s v="Tradepoint Atlantic"/>
+    <x v="14"/>
+    <x v="8"/>
     <x v="2"/>
     <s v="South Atlantic"/>
     <n v="2021"/>
@@ -3043,9 +3256,9 @@
   </r>
   <r>
     <s v="Jacket"/>
-    <x v="12"/>
-    <s v="Port of New Orleans"/>
-    <x v="7"/>
+    <x v="15"/>
+    <x v="11"/>
+    <x v="9"/>
     <s v="Gulf of Mexico"/>
     <n v="2023"/>
     <n v="3"/>
@@ -3055,10 +3268,23 @@
     <n v="3"/>
   </r>
   <r>
+    <s v="GBF"/>
+    <x v="16"/>
+    <x v="12"/>
+    <x v="1"/>
+    <s v="South Atlantic"/>
+    <n v="2025"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="2028"/>
+    <n v="3"/>
+  </r>
+  <r>
     <s v="Transition piece"/>
-    <x v="13"/>
-    <s v="Port of Albany"/>
-    <x v="4"/>
+    <x v="17"/>
+    <x v="7"/>
+    <x v="6"/>
     <s v="Central Atlantic"/>
     <n v="2021"/>
     <n v="3"/>
@@ -3069,9 +3295,9 @@
   </r>
   <r>
     <m/>
-    <x v="14"/>
-    <s v="Port of Coeymans"/>
-    <x v="4"/>
+    <x v="18"/>
+    <x v="13"/>
+    <x v="6"/>
     <s v="Central Atlantic"/>
     <n v="2023"/>
     <n v="3"/>
@@ -3082,9 +3308,9 @@
   </r>
   <r>
     <s v="Array cable"/>
-    <x v="15"/>
-    <s v="Tradepoint Atlantic"/>
-    <x v="5"/>
+    <x v="19"/>
+    <x v="8"/>
+    <x v="7"/>
     <s v="South Atlantic"/>
     <n v="2021"/>
     <n v="3"/>
@@ -3095,35 +3321,35 @@
   </r>
   <r>
     <m/>
-    <x v="16"/>
-    <s v="Arthur Kill Terminal"/>
-    <x v="4"/>
+    <x v="20"/>
+    <x v="14"/>
+    <x v="6"/>
     <s v="Central Atlantic"/>
     <n v="2023"/>
     <n v="3"/>
     <n v="5"/>
-    <n v="0.2"/>
-    <n v="2030"/>
-    <n v="7"/>
+    <n v="0.25"/>
+    <n v="2029"/>
+    <n v="6"/>
   </r>
   <r>
     <m/>
-    <x v="17"/>
-    <s v="Mystic River, Everett"/>
-    <x v="8"/>
+    <x v="21"/>
+    <x v="15"/>
+    <x v="10"/>
     <s v="North Atlantic"/>
     <n v="2023"/>
     <n v="3"/>
-    <n v="3"/>
+    <n v="5"/>
     <n v="0.25"/>
-    <n v="2028"/>
-    <n v="5"/>
+    <n v="2029"/>
+    <n v="6"/>
   </r>
   <r>
     <s v="Export cable"/>
-    <x v="18"/>
-    <s v="Goose Island"/>
-    <x v="9"/>
+    <x v="22"/>
+    <x v="16"/>
+    <x v="11"/>
     <s v="South Atlantic"/>
     <n v="2018"/>
     <n v="3"/>
@@ -3134,9 +3360,9 @@
   </r>
   <r>
     <m/>
-    <x v="19"/>
-    <s v="Brayton Point"/>
-    <x v="8"/>
+    <x v="23"/>
+    <x v="17"/>
+    <x v="10"/>
     <s v="North Atlantic"/>
     <n v="2021"/>
     <n v="3"/>
@@ -3147,9 +3373,9 @@
   </r>
   <r>
     <m/>
-    <x v="20"/>
-    <s v="Quonset Business Park / Port of Davisville"/>
-    <x v="3"/>
+    <x v="24"/>
+    <x v="18"/>
+    <x v="4"/>
     <s v="North Atlantic"/>
     <n v="2023"/>
     <n v="3"/>
@@ -3160,9 +3386,9 @@
   </r>
   <r>
     <m/>
-    <x v="21"/>
-    <s v="Radio Island, Morehead City"/>
-    <x v="1"/>
+    <x v="25"/>
+    <x v="19"/>
+    <x v="11"/>
     <s v="South Atlantic"/>
     <n v="2023"/>
     <n v="3"/>
@@ -3173,9 +3399,9 @@
   </r>
   <r>
     <s v="Steel plates"/>
-    <x v="22"/>
-    <s v="Brandenburg "/>
-    <x v="10"/>
+    <x v="26"/>
+    <x v="20"/>
+    <x v="12"/>
     <s v="South Atlantic"/>
     <n v="2021"/>
     <n v="3"/>
@@ -3186,9 +3412,9 @@
   </r>
   <r>
     <m/>
-    <x v="23"/>
-    <s v="Port of Brunswick"/>
-    <x v="11"/>
+    <x v="27"/>
+    <x v="21"/>
+    <x v="13"/>
     <s v="South Atlantic"/>
     <n v="2023"/>
     <n v="3"/>
@@ -3197,58 +3423,195 @@
     <n v="2029"/>
     <n v="6"/>
   </r>
+  <r>
+    <s v="Casting"/>
+    <x v="28"/>
+    <x v="22"/>
+    <x v="14"/>
+    <s v="Other"/>
+    <n v="2023"/>
+    <n v="0"/>
+    <n v="2"/>
+    <n v="0"/>
+    <n v="2025"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="Flange"/>
+    <x v="29"/>
+    <x v="23"/>
+    <x v="15"/>
+    <s v="North Atlantic"/>
+    <n v="2023"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="0.25"/>
+    <n v="2027"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <s v="Semisubmersible"/>
+    <x v="30"/>
+    <x v="6"/>
+    <x v="5"/>
+    <s v="West Coast"/>
+    <n v="2024"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="0.25"/>
+    <n v="2028"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <m/>
+    <x v="31"/>
+    <x v="24"/>
+    <x v="5"/>
+    <s v="West Coast"/>
+    <n v="2025"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="0.25"/>
+    <n v="2029"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <m/>
+    <x v="32"/>
+    <x v="4"/>
+    <x v="3"/>
+    <s v="West Coast"/>
+    <n v="2026"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="0.25"/>
+    <n v="2030"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <s v="Stationkeeping"/>
+    <x v="33"/>
+    <x v="25"/>
+    <x v="16"/>
+    <s v="West Coast"/>
+    <n v="2024"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="0.25"/>
+    <n v="2028"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <m/>
+    <x v="34"/>
+    <x v="25"/>
+    <x v="16"/>
+    <s v="West Coast"/>
+    <n v="2024"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="0.25"/>
+    <n v="2028"/>
+    <n v="4"/>
+  </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{391C8580-0FAE-4DE9-AE5F-736ACC565C2E}" name="PivotTable5" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
-  <location ref="G37:H50" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5CA5F775-FB12-4A7B-98B7-3842EC7091C4}" name="PivotTable1" cacheId="17" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
+  <location ref="G48:H66" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0">
-      <items count="25">
-        <item x="16"/>
-        <item x="17"/>
+      <items count="36">
+        <item x="20"/>
+        <item x="21"/>
         <item x="1"/>
         <item x="2"/>
         <item x="3"/>
+        <item x="4"/>
+        <item x="28"/>
+        <item x="13"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="29"/>
+        <item x="16"/>
+        <item x="5"/>
+        <item x="19"/>
+        <item x="15"/>
+        <item x="9"/>
+        <item x="33"/>
+        <item x="34"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="22"/>
+        <item x="26"/>
+        <item x="23"/>
+        <item x="30"/>
+        <item x="31"/>
+        <item x="32"/>
+        <item x="0"/>
+        <item x="17"/>
+        <item x="27"/>
         <item x="10"/>
-        <item x="20"/>
-        <item x="21"/>
-        <item x="4"/>
-        <item x="15"/>
+        <item x="11"/>
         <item x="12"/>
-        <item x="7"/>
+        <item x="18"/>
+        <item x="14"/>
         <item x="6"/>
-        <item x="18"/>
-        <item x="22"/>
-        <item x="19"/>
-        <item x="0"/>
-        <item x="13"/>
-        <item x="23"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="14"/>
-        <item x="11"/>
-        <item x="5"/>
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="27">
+        <item x="14"/>
+        <item x="20"/>
+        <item x="17"/>
+        <item x="19"/>
+        <item x="1"/>
+        <item x="16"/>
+        <item x="15"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="7"/>
+        <item x="21"/>
+        <item x="13"/>
+        <item x="11"/>
+        <item x="10"/>
+        <item x="0"/>
+        <item x="18"/>
+        <item x="12"/>
+        <item x="23"/>
+        <item x="9"/>
+        <item x="5"/>
+        <item x="24"/>
+        <item x="4"/>
+        <item x="6"/>
+        <item x="25"/>
+        <item x="8"/>
+        <item x="22"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
     <pivotField axis="axisRow" showAll="0">
-      <items count="13">
-        <item x="11"/>
+      <items count="18">
+        <item x="5"/>
+        <item x="13"/>
+        <item x="12"/>
+        <item x="9"/>
         <item x="10"/>
         <item x="7"/>
         <item x="8"/>
-        <item x="5"/>
+        <item x="1"/>
+        <item x="15"/>
+        <item x="2"/>
         <item x="6"/>
-        <item x="1"/>
-        <item x="2"/>
+        <item x="3"/>
+        <item x="14"/>
         <item x="4"/>
-        <item x="3"/>
-        <item x="9"/>
+        <item x="11"/>
         <item x="0"/>
+        <item x="16"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -3263,7 +3626,7 @@
   <rowFields count="1">
     <field x="3"/>
   </rowFields>
-  <rowItems count="13">
+  <rowItems count="18">
     <i>
       <x/>
     </i>
@@ -3300,6 +3663,21 @@
     <i>
       <x v="11"/>
     </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
     <i t="grand">
       <x/>
     </i>
@@ -3311,7 +3689,7 @@
     <dataField name="Count of Factory" fld="1" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <chartFormats count="1">
-    <chartFormat chart="0" format="0" series="1">
+    <chartFormat chart="1" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -3618,22 +3996,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F1FF48-4396-4FE3-ABD9-234FB66F60F4}">
-  <dimension ref="A1:L50"/>
+  <dimension ref="A1:L66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L57" sqref="L57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" customWidth="1"/>
     <col min="3" max="3" width="42.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.28515625" bestFit="1" customWidth="1"/>
@@ -3642,21 +4020,21 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" t="s">
         <v>96</v>
-      </c>
-      <c r="B3" t="s">
-        <v>97</v>
       </c>
       <c r="C3">
         <v>0.25</v>
       </c>
       <c r="D3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -3667,18 +4045,18 @@
         <v>2023</v>
       </c>
       <c r="D4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C5">
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -3791,14 +4169,14 @@
         <v>2023</v>
       </c>
       <c r="G10">
-        <f t="shared" ref="G10:G33" si="0">$C$5</f>
+        <f t="shared" ref="G10:G36" si="0">$C$5</f>
         <v>3</v>
       </c>
       <c r="H10">
         <v>3</v>
       </c>
       <c r="I10">
-        <f t="shared" ref="I10:I12" si="1">$C$3</f>
+        <f t="shared" ref="I10:I13" si="1">$C$3</f>
         <v>0.25</v>
       </c>
       <c r="J10">
@@ -3806,7 +4184,7 @@
         <v>2028</v>
       </c>
       <c r="K10">
-        <f t="shared" ref="K10:K33" si="2">J10-F10</f>
+        <f t="shared" ref="K10:K43" si="2">J10-F10</f>
         <v>5</v>
       </c>
       <c r="L10" t="s">
@@ -3841,7 +4219,7 @@
         <v>0.25</v>
       </c>
       <c r="J11">
-        <f t="shared" ref="J11:J33" si="3">ROUNDDOWN(F11+G11+H11*(1-I11),0)</f>
+        <f t="shared" ref="J11:J43" si="3">ROUNDDOWN(F11+G11+H11*(1-I11),0)</f>
         <v>2028</v>
       </c>
       <c r="K11">
@@ -3892,50 +4270,46 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>50</v>
-      </c>
       <c r="B13" t="s">
-        <v>51</v>
-      </c>
-      <c r="C13" t="s">
-        <v>48</v>
+        <v>123</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>131</v>
       </c>
       <c r="D13" t="s">
-        <v>27</v>
+        <v>127</v>
       </c>
       <c r="E13" t="s">
-        <v>25</v>
+        <v>128</v>
       </c>
       <c r="F13">
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="G13">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H13">
         <v>3</v>
       </c>
       <c r="I13">
-        <f>1/3</f>
-        <v>0.33333333333333331</v>
+        <f t="shared" si="1"/>
+        <v>0.25</v>
       </c>
       <c r="J13">
         <f t="shared" si="3"/>
-        <v>2026</v>
+        <v>2030</v>
       </c>
       <c r="K13">
         <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="L13" t="s">
-        <v>99</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>50</v>
+      </c>
       <c r="B14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C14" t="s">
         <v>48</v>
@@ -3969,24 +4343,24 @@
         <v>5</v>
       </c>
       <c r="L14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>30</v>
+        <v>52</v>
+      </c>
+      <c r="C15" t="s">
+        <v>48</v>
       </c>
       <c r="D15" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="E15" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="F15">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="G15">
         <f t="shared" si="0"/>
@@ -3996,113 +4370,109 @@
         <v>3</v>
       </c>
       <c r="I15">
-        <f t="shared" ref="I15" si="4">$C$3</f>
-        <v>0.25</v>
+        <f>1/3</f>
+        <v>0.33333333333333331</v>
       </c>
       <c r="J15">
         <f t="shared" si="3"/>
-        <v>2028</v>
+        <v>2026</v>
       </c>
       <c r="K15">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
+      <c r="L15" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>54</v>
-      </c>
       <c r="B16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D16" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E16" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="F16">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="G16">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="H16">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="I16">
-        <v>0.8</v>
+        <f t="shared" ref="I16" si="4">$C$3</f>
+        <v>0.25</v>
       </c>
       <c r="J16">
         <f t="shared" si="3"/>
-        <v>2024</v>
+        <v>2028</v>
       </c>
       <c r="K16">
         <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="L16" t="s">
-        <v>100</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>57</v>
+        <v>125</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>58</v>
+        <v>129</v>
       </c>
       <c r="D17" t="s">
-        <v>6</v>
+        <v>124</v>
       </c>
       <c r="E17" t="s">
-        <v>5</v>
+        <v>128</v>
       </c>
       <c r="F17">
         <v>2023</v>
       </c>
       <c r="G17">
-        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H17">
         <v>3</v>
       </c>
-      <c r="H17">
-        <v>2.5</v>
-      </c>
       <c r="I17">
-        <f t="shared" ref="I17:I18" si="5">$C$3</f>
         <v>0.25</v>
       </c>
       <c r="J17">
-        <f t="shared" si="3"/>
-        <v>2027</v>
+        <f t="shared" ref="J17" si="5">ROUNDDOWN(F17+G17+H17*(1-I17),0)</f>
+        <v>2029</v>
       </c>
       <c r="K17">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="L17" t="s">
-        <v>59</v>
+        <f t="shared" ref="K17" si="6">J17-F17</f>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>54</v>
+      </c>
       <c r="B18" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="D18" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E18" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="F18">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="G18">
         <f t="shared" si="0"/>
@@ -4112,198 +4482,186 @@
         <v>2.5</v>
       </c>
       <c r="I18">
-        <f t="shared" si="5"/>
-        <v>0.25</v>
+        <v>0.8</v>
       </c>
       <c r="J18">
         <f t="shared" si="3"/>
-        <v>2027</v>
+        <v>2024</v>
       </c>
       <c r="K18">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L18" t="s">
-        <v>61</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>62</v>
-      </c>
       <c r="B19" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="D19" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="E19" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="F19">
-        <v>2020</v>
+        <v>2023</v>
       </c>
       <c r="G19">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="H19">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="I19">
-        <v>0.5</v>
+        <f t="shared" ref="I19:I21" si="7">$C$3</f>
+        <v>0.25</v>
       </c>
       <c r="J19">
         <f t="shared" si="3"/>
-        <v>2024</v>
+        <v>2027</v>
       </c>
       <c r="K19">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="L19" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>58</v>
+        <v>19</v>
       </c>
       <c r="D20" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="E20" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="F20">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="G20">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="H20">
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
       <c r="I20">
-        <f t="shared" ref="I20:I21" si="6">$C$3</f>
+        <f t="shared" si="7"/>
         <v>0.25</v>
       </c>
       <c r="J20">
         <f t="shared" si="3"/>
-        <v>2026</v>
+        <v>2027</v>
       </c>
       <c r="K20">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L20" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>66</v>
-      </c>
       <c r="B21" t="s">
-        <v>67</v>
+        <v>126</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>22</v>
+        <v>129</v>
       </c>
       <c r="D21" t="s">
-        <v>23</v>
+        <v>124</v>
       </c>
       <c r="E21" t="s">
-        <v>68</v>
+        <v>128</v>
       </c>
       <c r="F21">
         <v>2023</v>
       </c>
       <c r="G21">
+        <v>4</v>
+      </c>
+      <c r="H21">
+        <v>2.5</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="7"/>
+        <v>0.25</v>
+      </c>
+      <c r="J21">
+        <f t="shared" ref="J21" si="8">ROUNDDOWN(F21+G21+H21*(1-I21),0)</f>
+        <v>2028</v>
+      </c>
+      <c r="K21">
+        <f t="shared" ref="K21" si="9">J21-F21</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22">
+        <v>2020</v>
+      </c>
+      <c r="G22">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="H21">
-        <v>1</v>
-      </c>
-      <c r="I21">
-        <f t="shared" si="6"/>
-        <v>0.25</v>
-      </c>
-      <c r="J21">
-        <f>ROUNDDOWN(F21+G21+H21*(1-I21),0)</f>
-        <v>2026</v>
-      </c>
-      <c r="K21">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="L21" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>108</v>
-      </c>
-      <c r="B22" t="s">
-        <v>109</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="D22" t="s">
-        <v>10</v>
-      </c>
-      <c r="E22" t="s">
-        <v>5</v>
-      </c>
-      <c r="F22">
-        <v>2025</v>
-      </c>
-      <c r="G22">
+      <c r="H22">
         <v>2</v>
       </c>
-      <c r="H22">
-        <v>1</v>
-      </c>
       <c r="I22">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="J22">
-        <f>ROUNDDOWN(F22+G22+H22*(1-I22),0)</f>
-        <v>2028</v>
+        <f t="shared" si="3"/>
+        <v>2024</v>
       </c>
       <c r="K22">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L22" t="s">
-        <v>110</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>70</v>
-      </c>
       <c r="B23" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="D23" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E23" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="F23">
         <v>2021</v>
@@ -4313,35 +4671,39 @@
         <v>3</v>
       </c>
       <c r="H23">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
       <c r="I23">
+        <f t="shared" ref="I23:I24" si="10">$C$3</f>
         <v>0.25</v>
       </c>
       <c r="J23">
         <f t="shared" si="3"/>
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="K23">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L23" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>66</v>
+      </c>
       <c r="B24" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>73</v>
+        <v>22</v>
       </c>
       <c r="D24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E24" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="F24">
         <v>2023</v>
@@ -4351,69 +4713,73 @@
         <v>3</v>
       </c>
       <c r="H24">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="I24">
-        <f t="shared" ref="I24:I26" si="7">$C$3</f>
+        <f t="shared" si="10"/>
         <v>0.25</v>
       </c>
       <c r="J24">
-        <f t="shared" si="3"/>
-        <v>2027</v>
+        <f>ROUNDDOWN(F24+G24+H24*(1-I24),0)</f>
+        <v>2026</v>
       </c>
       <c r="K24">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L24" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>75</v>
+        <v>107</v>
       </c>
       <c r="B25" t="s">
-        <v>76</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>58</v>
+        <v>108</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>88</v>
       </c>
       <c r="D25" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E25" t="s">
         <v>5</v>
       </c>
       <c r="F25">
-        <v>2021</v>
+        <v>2025</v>
       </c>
       <c r="G25">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H25">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I25">
-        <f t="shared" si="7"/>
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="J25">
-        <f t="shared" si="3"/>
-        <v>2027</v>
+        <f>ROUNDDOWN(F25+G25+H25*(1-I25),0)</f>
+        <v>2028</v>
       </c>
       <c r="K25">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="L25" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>70</v>
+      </c>
       <c r="B26" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D26" t="s">
         <v>24</v>
@@ -4422,43 +4788,42 @@
         <v>25</v>
       </c>
       <c r="F26">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="G26">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="H26">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="I26">
-        <f t="shared" si="7"/>
         <v>0.25</v>
       </c>
       <c r="J26">
         <f t="shared" si="3"/>
-        <v>2029</v>
+        <v>2025</v>
       </c>
       <c r="K26">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L26" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>79</v>
+        <v>110</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>21</v>
+        <v>72</v>
       </c>
       <c r="D27" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="E27" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="F27">
         <v>2023</v>
@@ -4468,76 +4833,78 @@
         <v>3</v>
       </c>
       <c r="H27">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="I27">
-        <f t="shared" ref="I27" si="8">$C$3</f>
+        <f t="shared" ref="I27:I29" si="11">$C$3</f>
         <v>0.25</v>
       </c>
       <c r="J27">
         <f t="shared" si="3"/>
-        <v>2029</v>
+        <v>2027</v>
       </c>
       <c r="K27">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="L27" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B28" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="D28" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="E28" t="s">
         <v>5</v>
       </c>
       <c r="F28">
-        <v>2018</v>
+        <v>2021</v>
       </c>
       <c r="G28">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="H28" t="s">
-        <v>83</v>
-      </c>
-      <c r="I28" t="s">
-        <v>83</v>
+      <c r="H28">
+        <v>5</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="11"/>
+        <v>0.25</v>
       </c>
       <c r="J28">
-        <v>2020</v>
+        <f t="shared" si="3"/>
+        <v>2027</v>
       </c>
       <c r="K28">
         <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="L28" t="s">
-        <v>84</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="D29" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="E29" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="F29">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="G29">
         <f t="shared" si="0"/>
@@ -4547,27 +4914,30 @@
         <v>5</v>
       </c>
       <c r="I29">
-        <f t="shared" ref="I29:I33" si="9">$C$3</f>
+        <f t="shared" si="11"/>
         <v>0.25</v>
       </c>
       <c r="J29">
         <f t="shared" si="3"/>
-        <v>2027</v>
+        <v>2029</v>
       </c>
       <c r="K29">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
+      <c r="L29" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>86</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>17</v>
+        <v>78</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="D30" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E30" t="s">
         <v>16</v>
@@ -4583,7 +4953,7 @@
         <v>5</v>
       </c>
       <c r="I30">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="I30" si="12">$C$3</f>
         <v>0.25</v>
       </c>
       <c r="J30">
@@ -4594,16 +4964,16 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="L30" t="s">
-        <v>87</v>
-      </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>79</v>
+      </c>
       <c r="B31" t="s">
-        <v>88</v>
-      </c>
-      <c r="C31" t="s">
-        <v>12</v>
+        <v>80</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="D31" t="s">
         <v>13</v>
@@ -4612,43 +4982,41 @@
         <v>5</v>
       </c>
       <c r="F31">
-        <v>2023</v>
+        <v>2018</v>
       </c>
       <c r="G31">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="H31">
-        <v>5</v>
-      </c>
-      <c r="I31">
-        <f t="shared" si="9"/>
-        <v>0.25</v>
+      <c r="H31" t="s">
+        <v>82</v>
+      </c>
+      <c r="I31" t="s">
+        <v>82</v>
       </c>
       <c r="J31">
-        <f t="shared" si="3"/>
-        <v>2029</v>
+        <v>2020</v>
       </c>
       <c r="K31">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>2</v>
+      </c>
+      <c r="L31" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>90</v>
-      </c>
       <c r="B32" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>92</v>
+        <v>14</v>
       </c>
       <c r="D32" t="s">
-        <v>93</v>
+        <v>15</v>
       </c>
       <c r="E32" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="F32">
         <v>2021</v>
@@ -4658,33 +5026,33 @@
         <v>3</v>
       </c>
       <c r="H32">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I32">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="I32:I36" si="13">$C$3</f>
         <v>0.25</v>
       </c>
       <c r="J32">
         <f t="shared" si="3"/>
-        <v>2025</v>
+        <v>2027</v>
       </c>
       <c r="K32">
         <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>94</v>
-      </c>
-      <c r="C33" t="s">
-        <v>3</v>
+        <v>85</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="D33" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="E33" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="F33">
         <v>2023</v>
@@ -4697,7 +5065,7 @@
         <v>5</v>
       </c>
       <c r="I33">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0.25</v>
       </c>
       <c r="J33">
@@ -4708,125 +5076,539 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+      <c r="L33" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>87</v>
+      </c>
+      <c r="C34" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" t="s">
+        <v>13</v>
+      </c>
+      <c r="E34" t="s">
+        <v>5</v>
+      </c>
+      <c r="F34">
+        <v>2023</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H34">
+        <v>5</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="13"/>
+        <v>0.25</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="3"/>
+        <v>2029</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>89</v>
+      </c>
+      <c r="B35" t="s">
+        <v>90</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D35" t="s">
+        <v>92</v>
+      </c>
+      <c r="E35" t="s">
+        <v>5</v>
+      </c>
+      <c r="F35">
+        <v>2021</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H35">
+        <v>2</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="13"/>
+        <v>0.25</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="3"/>
+        <v>2025</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>93</v>
+      </c>
+      <c r="C36" t="s">
+        <v>3</v>
+      </c>
+      <c r="D36" t="s">
+        <v>4</v>
+      </c>
+      <c r="E36" t="s">
+        <v>5</v>
+      </c>
+      <c r="F36">
+        <v>2023</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H36">
+        <v>5</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="13"/>
+        <v>0.25</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="3"/>
+        <v>2029</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>111</v>
+      </c>
+      <c r="B37" t="s">
+        <v>112</v>
+      </c>
+      <c r="D37" t="s">
+        <v>113</v>
+      </c>
+      <c r="E37" t="s">
+        <v>114</v>
+      </c>
+      <c r="F37">
+        <v>2023</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>2</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="3"/>
+        <v>2025</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="L37" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>135</v>
+      </c>
+      <c r="B38" t="s">
+        <v>136</v>
+      </c>
+      <c r="C38" t="s">
+        <v>138</v>
+      </c>
+      <c r="D38" t="s">
+        <v>137</v>
+      </c>
+      <c r="E38" t="s">
+        <v>16</v>
+      </c>
+      <c r="F38">
+        <v>2023</v>
+      </c>
+      <c r="G38">
+        <v>3</v>
+      </c>
+      <c r="H38">
+        <v>2</v>
+      </c>
+      <c r="I38">
+        <v>0.25</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="3"/>
+        <v>2027</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>116</v>
+      </c>
+      <c r="B39" t="s">
+        <v>117</v>
+      </c>
+      <c r="C39" t="s">
+        <v>129</v>
+      </c>
+      <c r="D39" t="s">
+        <v>124</v>
+      </c>
+      <c r="E39" t="s">
+        <v>128</v>
+      </c>
+      <c r="F39">
+        <v>2024</v>
+      </c>
+      <c r="G39">
+        <v>4</v>
+      </c>
+      <c r="H39">
+        <v>1</v>
+      </c>
+      <c r="I39">
+        <v>0.25</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="3"/>
+        <v>2028</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="L39" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>118</v>
+      </c>
+      <c r="C40" t="s">
+        <v>130</v>
+      </c>
+      <c r="D40" t="s">
+        <v>124</v>
+      </c>
+      <c r="E40" t="s">
+        <v>128</v>
+      </c>
+      <c r="F40">
+        <v>2025</v>
+      </c>
+      <c r="G40">
+        <v>4</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
+      <c r="I40">
+        <v>0.25</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="3"/>
+        <v>2029</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="L40" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>119</v>
+      </c>
+      <c r="C41" t="s">
+        <v>131</v>
+      </c>
+      <c r="D41" t="s">
+        <v>127</v>
+      </c>
+      <c r="E41" t="s">
+        <v>128</v>
+      </c>
+      <c r="F41">
+        <v>2026</v>
+      </c>
+      <c r="G41">
+        <v>4</v>
+      </c>
+      <c r="H41">
+        <v>1</v>
+      </c>
+      <c r="I41">
+        <v>0.25</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="3"/>
+        <v>2030</v>
+      </c>
+      <c r="K41">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="L41" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>120</v>
+      </c>
+      <c r="B42" t="s">
+        <v>121</v>
+      </c>
+      <c r="C42" t="s">
+        <v>132</v>
+      </c>
+      <c r="D42" t="s">
+        <v>133</v>
+      </c>
+      <c r="E42" t="s">
+        <v>128</v>
+      </c>
+      <c r="F42">
+        <v>2024</v>
+      </c>
+      <c r="G42">
+        <v>3</v>
+      </c>
+      <c r="H42">
+        <v>2</v>
+      </c>
+      <c r="I42">
+        <v>0.25</v>
+      </c>
+      <c r="J42">
+        <f t="shared" si="3"/>
+        <v>2028</v>
+      </c>
+      <c r="K42">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>122</v>
+      </c>
+      <c r="C43" t="s">
+        <v>132</v>
+      </c>
+      <c r="D43" t="s">
+        <v>133</v>
+      </c>
+      <c r="E43" t="s">
+        <v>128</v>
+      </c>
+      <c r="F43">
+        <v>2024</v>
+      </c>
+      <c r="G43">
+        <v>3</v>
+      </c>
+      <c r="H43">
+        <v>2</v>
+      </c>
+      <c r="I43">
+        <v>0.25</v>
+      </c>
+      <c r="J43">
+        <f t="shared" si="3"/>
+        <v>2028</v>
+      </c>
+      <c r="K43">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G48" s="6" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G37" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="H37" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G38" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="H38" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G39" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="H39" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G40" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H40" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G41" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H41" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G42" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="H42" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G43" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H43" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G44" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="H44" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G45" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H45" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G46" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H46" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G47" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H47" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G48" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H48" s="8">
-        <v>1</v>
+      <c r="H48" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="49" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G49" s="7" t="s">
-        <v>8</v>
+        <v>124</v>
       </c>
       <c r="H49" s="8">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G50" s="7" t="s">
-        <v>106</v>
+        <v>4</v>
       </c>
       <c r="H50" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G51" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="H51" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G52" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H52" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G53" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H53" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G54" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H54" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G55" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H55" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G56" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H56" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G57" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="H57" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G58" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H58" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G59" s="7" t="s">
         <v>24</v>
       </c>
+      <c r="H59" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G60" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="H60" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G61" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="H61" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G62" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H62" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G63" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H63" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G64" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H64" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G65" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="H65" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G66" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="H66" s="8">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
   <drawing r:id="rId3"/>

</xml_diff>

<commit_message>
Initial draft of overall gantt.  Revisions to floating
</commit_message>
<xml_diff>
--- a/fabrication_ports/ports_scenario.xlsx
+++ b/fabrication_ports/ports_scenario.xlsx
@@ -2,22 +2,25 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
-  <workbookPr/>
+  <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mshields\Documents\Projects\Supply Chain Roadmap\Analysis repos\Roadmap\fabrication_ports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD9F57B-1AA3-4966-8420-9368CD77A6AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{141152F6-F16F-4E22-B02C-323EF077D558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Avg Demand Scenario" sheetId="9" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Avg Demand Scenario'!$E$8:$E$46</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="17" r:id="rId2"/>
+    <pivotCache cacheId="24" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="176">
   <si>
     <t>Port</t>
   </si>
@@ -70,9 +73,6 @@
     <t>NC</t>
   </si>
   <si>
-    <t>Newport News Marine Terminal</t>
-  </si>
-  <si>
     <t>Columbus Terminal</t>
   </si>
   <si>
@@ -271,9 +271,6 @@
     <t>AKT expected to be ready for operations in 2026</t>
   </si>
   <si>
-    <t>Array cable 2</t>
-  </si>
-  <si>
     <t>Export cable</t>
   </si>
   <si>
@@ -439,9 +436,6 @@
     <t>WA</t>
   </si>
   <si>
-    <t>Assume fabricaiton elsewhere (GOM, Asia) and assembly at marshalling site.  Somewhat industrialized.  Don't need major facility upgrades (beyond port fab)</t>
-  </si>
-  <si>
     <t>Flange</t>
   </si>
   <si>
@@ -452,6 +446,126 @@
   </si>
   <si>
     <t>Schiller Newington, Portsmouth</t>
+  </si>
+  <si>
+    <t>Semisubmersible 4</t>
+  </si>
+  <si>
+    <t>Assembly port</t>
+  </si>
+  <si>
+    <t>Fabrication shipyard(new build)</t>
+  </si>
+  <si>
+    <t>Semisubmersible 5</t>
+  </si>
+  <si>
+    <t>TBD - TX</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>Fabrication shipyard (expand exising facility)</t>
+  </si>
+  <si>
+    <t>TBD - LA</t>
+  </si>
+  <si>
+    <t>Semisubmersible 6</t>
+  </si>
+  <si>
+    <t>Semisubmersible 7</t>
+  </si>
+  <si>
+    <t>Service WC and EC</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Mystic River, MA</t>
+  </si>
+  <si>
+    <t>Coos Bay, OR</t>
+  </si>
+  <si>
+    <t>New Jersey Wind Port, NJ</t>
+  </si>
+  <si>
+    <t>Portsmouth Marine Terminal, VA</t>
+  </si>
+  <si>
+    <t>Port of Wilmington, NC</t>
+  </si>
+  <si>
+    <t>South Quay, RI</t>
+  </si>
+  <si>
+    <t>Port of Humboldt, CA</t>
+  </si>
+  <si>
+    <t>Port of Albany, NY</t>
+  </si>
+  <si>
+    <t>Tradepoint Atlantic, MD</t>
+  </si>
+  <si>
+    <t>Searsport, ME</t>
+  </si>
+  <si>
+    <t>Port of Paulsboro, NJ</t>
+  </si>
+  <si>
+    <t>Port of New Orleans, LA</t>
+  </si>
+  <si>
+    <t>Radio Island, NC</t>
+  </si>
+  <si>
+    <t>Port of Coeymans, NY</t>
+  </si>
+  <si>
+    <t>Arthur Kill Terminal, NY</t>
+  </si>
+  <si>
+    <t>Goose Island, SC</t>
+  </si>
+  <si>
+    <t>Brayton Point, MA</t>
+  </si>
+  <si>
+    <t>Quonset Business Park, RI</t>
+  </si>
+  <si>
+    <t>Port of Charlotte, SC</t>
+  </si>
+  <si>
+    <t>Brandenburg, KY</t>
+  </si>
+  <si>
+    <t>Port of Brunswick, GA</t>
+  </si>
+  <si>
+    <t>Inland facility, PA</t>
+  </si>
+  <si>
+    <t>Portsmouth, NH</t>
+  </si>
+  <si>
+    <t>Central Coast, CA</t>
+  </si>
+  <si>
+    <t>WA shipyard, WA</t>
+  </si>
+  <si>
+    <t>TX shipyard, TX</t>
+  </si>
+  <si>
+    <t>TX port, TX</t>
+  </si>
+  <si>
+    <t>LA port, LA</t>
   </si>
 </sst>
 </file>
@@ -655,7 +769,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Avg Demand Scenario'!$F$8</c:f>
+              <c:f>'Avg Demand Scenario'!$G$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -674,9 +788,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Avg Demand Scenario'!$B$9:$B$36</c:f>
+              <c:f>'Avg Demand Scenario'!$B$9:$B$35</c:f>
               <c:strCache>
-                <c:ptCount val="28"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>SGRE</c:v>
                 </c:pt>
@@ -741,24 +855,21 @@
                   <c:v>Array cable 1</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>Array cable 2</c:v>
+                  <c:v>Nexans</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>Nexans</c:v>
+                  <c:v>Prysmian</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>Prysmian</c:v>
+                  <c:v>Export cable 1</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>Export cable 1</c:v>
+                  <c:v>Export cable 2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>Export cable 2</c:v>
+                  <c:v>Nucor</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>Nucor</c:v>
-                </c:pt>
-                <c:pt idx="27">
                   <c:v>Steel plate 1</c:v>
                 </c:pt>
               </c:strCache>
@@ -766,10 +877,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Avg Demand Scenario'!$F$9:$F$36</c:f>
+              <c:f>'Avg Demand Scenario'!$G$9:$G$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>2021</c:v>
                 </c:pt>
@@ -834,24 +945,21 @@
                   <c:v>2023</c:v>
                 </c:pt>
                 <c:pt idx="21">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="23">
                   <c:v>2023</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>2018</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>2021</c:v>
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>2023</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2023</c:v>
+                  <c:v>2021</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2021</c:v>
-                </c:pt>
-                <c:pt idx="27">
                   <c:v>2023</c:v>
                 </c:pt>
               </c:numCache>
@@ -868,7 +976,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Avg Demand Scenario'!$K$8</c:f>
+              <c:f>'Avg Demand Scenario'!$L$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -889,9 +997,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Avg Demand Scenario'!$B$9:$B$36</c:f>
+              <c:f>'Avg Demand Scenario'!$B$9:$B$35</c:f>
               <c:strCache>
-                <c:ptCount val="28"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>SGRE</c:v>
                 </c:pt>
@@ -956,24 +1064,21 @@
                   <c:v>Array cable 1</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>Array cable 2</c:v>
+                  <c:v>Nexans</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>Nexans</c:v>
+                  <c:v>Prysmian</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>Prysmian</c:v>
+                  <c:v>Export cable 1</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>Export cable 1</c:v>
+                  <c:v>Export cable 2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>Export cable 2</c:v>
+                  <c:v>Nucor</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>Nucor</c:v>
-                </c:pt>
-                <c:pt idx="27">
                   <c:v>Steel plate 1</c:v>
                 </c:pt>
               </c:strCache>
@@ -981,10 +1086,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Avg Demand Scenario'!$K$9:$K$36</c:f>
+              <c:f>'Avg Demand Scenario'!$L$9:$L$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -1049,10 +1154,10 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="21">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>6</c:v>
@@ -1061,12 +1166,9 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>6</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="27">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -1400,7 +1502,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Avg Demand Scenario'!$H$48</c:f>
+              <c:f>'Avg Demand Scenario'!$I$51</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1421,9 +1523,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Avg Demand Scenario'!$G$49:$G$66</c:f>
+              <c:f>'Avg Demand Scenario'!$H$52:$H$70</c:f>
               <c:strCache>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>CA</c:v>
                 </c:pt>
@@ -1474,16 +1576,19 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>WA</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>TX</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Avg Demand Scenario'!$H$49:$H$66</c:f>
+              <c:f>'Avg Demand Scenario'!$I$52:$I$70</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>4</c:v>
                 </c:pt>
@@ -1494,7 +1599,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>2</c:v>
@@ -1530,9 +1635,12 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
@@ -2857,13 +2965,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>30254</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>58177</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>209736</xdr:colOff>
-      <xdr:row>77</xdr:row>
+      <xdr:row>80</xdr:row>
       <xdr:rowOff>75266</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2891,15 +2999,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>898921</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>75008</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>2458640</xdr:colOff>
-      <xdr:row>60</xdr:row>
+      <xdr:row>63</xdr:row>
       <xdr:rowOff>151208</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2929,85 +3037,22 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Shields, Matt" refreshedDate="44770.98404166667" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="35" xr:uid="{8520C2B9-52CF-46B0-8F6A-64DE6645DC34}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Shields, Matt" refreshedDate="44771.362389467591" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="39" xr:uid="{8520C2B9-52CF-46B0-8F6A-64DE6645DC34}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A8:K43" sheet="Avg Demand Scenario"/>
+    <worksheetSource ref="A8:L46" sheet="Avg Demand Scenario"/>
   </cacheSource>
   <cacheFields count="11">
     <cacheField name="Component" numFmtId="0">
       <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="Factory" numFmtId="0">
-      <sharedItems count="35">
-        <s v="SGRE"/>
-        <s v="Blade 1"/>
-        <s v="Blade 2"/>
-        <s v="Blade 3"/>
-        <s v="Blade 4"/>
-        <s v="GE"/>
-        <s v="Vestas"/>
-        <s v="Nacelle 1"/>
-        <s v="Nacelle 2"/>
-        <s v="Marmen Welcon"/>
-        <s v="Tower 1"/>
-        <s v="Tower 2"/>
-        <s v="Tower 3"/>
-        <s v="EEW"/>
-        <s v="US Wind"/>
-        <s v="Jacket 1"/>
-        <s v="GBF 1"/>
-        <s v="Smulders"/>
-        <s v="Transition piece 1"/>
-        <s v="Hellenic"/>
-        <s v="Array cable 1"/>
-        <s v="Array cable 2"/>
-        <s v="Nexans"/>
-        <s v="Prysmian"/>
-        <s v="Export cable 1"/>
-        <s v="Export cable 2"/>
-        <s v="Nucor"/>
-        <s v="Steel plate 1"/>
-        <s v="Casting 1"/>
-        <s v="Flange 1"/>
-        <s v="Semisubmersible 1"/>
-        <s v="Semisubmersible 2"/>
-        <s v="Semisubmersible 3"/>
-        <s v="Mooring chain 1"/>
-        <s v="Mooring rope 1"/>
-      </sharedItems>
+      <sharedItems/>
     </cacheField>
     <cacheField name="Port" numFmtId="0">
-      <sharedItems containsBlank="1" count="26">
-        <s v="Portsmouth Marine Terminal"/>
-        <s v="General Cargo Terminal at Port of Wilmington"/>
-        <s v="Newport News Marine Terminal"/>
-        <s v="New Jersey Wind Port"/>
-        <s v="TBD - Coos Bay"/>
-        <s v="South Quay"/>
-        <s v="TBD - Humboldt"/>
-        <s v="Port of Albany"/>
-        <s v="Tradepoint Atlantic"/>
-        <s v="Searsport"/>
-        <s v="Port of Paulsboro"/>
-        <s v="Port of New Orleans"/>
-        <s v="Radio Island, Morehead City"/>
-        <s v="Port of Coeymans"/>
-        <s v="Arthur Kill Terminal"/>
-        <s v="Mystic River, Everett"/>
-        <s v="Goose Island"/>
-        <s v="Brayton Point"/>
-        <s v="Quonset Business Park / Port of Davisville"/>
-        <s v="Columbus Terminal"/>
-        <s v="Brandenburg "/>
-        <s v="Port of Brunswick"/>
-        <m/>
-        <s v="Schiller Newington, Portsmouth"/>
-        <s v="TBD - Central Coast"/>
-        <s v="TBD - WA"/>
-      </sharedItems>
+      <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="State" numFmtId="0">
-      <sharedItems count="17">
+      <sharedItems count="18">
         <s v="VA"/>
         <s v="NC"/>
         <s v="NJ"/>
@@ -3025,13 +3070,14 @@
         <s v="PA"/>
         <s v="NH"/>
         <s v="WA"/>
+        <s v="TX"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Region" numFmtId="0">
       <sharedItems/>
     </cacheField>
     <cacheField name="Announcement date" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2018" maxValue="2026"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2018" maxValue="2031"/>
     </cacheField>
     <cacheField name="Port upgrade duration (yrs)" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="4"/>
@@ -3043,7 +3089,7 @@
       <sharedItems containsMixedTypes="1" containsNumber="1" minValue="0" maxValue="0.8"/>
     </cacheField>
     <cacheField name="Operational date" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2020" maxValue="2030"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2020" maxValue="2033"/>
     </cacheField>
     <cacheField name="Duration" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2" maxValue="6"/>
@@ -3058,11 +3104,11 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="35">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="39">
   <r>
     <s v="Blade"/>
-    <x v="0"/>
-    <x v="0"/>
+    <s v="SGRE"/>
+    <s v="Portsmouth Marine Terminal"/>
     <x v="0"/>
     <s v="South Atlantic"/>
     <n v="2021"/>
@@ -3074,8 +3120,8 @@
   </r>
   <r>
     <m/>
-    <x v="1"/>
-    <x v="1"/>
+    <s v="Blade 1"/>
+    <s v="General Cargo Terminal at Port of Wilmington"/>
     <x v="1"/>
     <s v="South Atlantic"/>
     <n v="2023"/>
@@ -3087,8 +3133,8 @@
   </r>
   <r>
     <m/>
-    <x v="2"/>
-    <x v="2"/>
+    <s v="Blade 2"/>
+    <s v="Newport News Marine Terminal"/>
     <x v="0"/>
     <s v="South Atlantic"/>
     <n v="2023"/>
@@ -3100,8 +3146,8 @@
   </r>
   <r>
     <m/>
-    <x v="3"/>
-    <x v="3"/>
+    <s v="Blade 3"/>
+    <s v="New Jersey Wind Port"/>
     <x v="2"/>
     <s v="Central Atlantic"/>
     <n v="2023"/>
@@ -3113,8 +3159,8 @@
   </r>
   <r>
     <m/>
-    <x v="4"/>
-    <x v="4"/>
+    <s v="Blade 4"/>
+    <s v="TBD - Coos Bay"/>
     <x v="3"/>
     <s v="West Coast"/>
     <n v="2024"/>
@@ -3126,8 +3172,8 @@
   </r>
   <r>
     <s v="Nacelle"/>
-    <x v="5"/>
-    <x v="3"/>
+    <s v="GE"/>
+    <s v="New Jersey Wind Port"/>
     <x v="2"/>
     <s v="Central Atlantic"/>
     <n v="2021"/>
@@ -3139,8 +3185,8 @@
   </r>
   <r>
     <m/>
-    <x v="6"/>
-    <x v="3"/>
+    <s v="Vestas"/>
+    <s v="New Jersey Wind Port"/>
     <x v="2"/>
     <s v="Central Atlantic"/>
     <n v="2021"/>
@@ -3152,8 +3198,8 @@
   </r>
   <r>
     <m/>
-    <x v="7"/>
-    <x v="5"/>
+    <s v="Nacelle 1"/>
+    <s v="South Quay"/>
     <x v="4"/>
     <s v="North Atlantic"/>
     <n v="2023"/>
@@ -3165,8 +3211,8 @@
   </r>
   <r>
     <m/>
-    <x v="8"/>
-    <x v="6"/>
+    <s v="Nacelle 2"/>
+    <s v="TBD - Humboldt"/>
     <x v="5"/>
     <s v="West Coast"/>
     <n v="2023"/>
@@ -3178,8 +3224,8 @@
   </r>
   <r>
     <s v="Tower"/>
-    <x v="9"/>
-    <x v="7"/>
+    <s v="Marmen Welcon"/>
+    <s v="Port of Albany"/>
     <x v="6"/>
     <s v="Central Atlantic"/>
     <n v="2021"/>
@@ -3191,8 +3237,8 @@
   </r>
   <r>
     <m/>
-    <x v="10"/>
-    <x v="8"/>
+    <s v="Tower 1"/>
+    <s v="Tradepoint Atlantic"/>
     <x v="7"/>
     <s v="South Atlantic"/>
     <n v="2023"/>
@@ -3204,8 +3250,8 @@
   </r>
   <r>
     <m/>
-    <x v="11"/>
-    <x v="9"/>
+    <s v="Tower 2"/>
+    <s v="Searsport"/>
     <x v="8"/>
     <s v="North Atlantic"/>
     <n v="2023"/>
@@ -3217,8 +3263,8 @@
   </r>
   <r>
     <m/>
-    <x v="12"/>
-    <x v="6"/>
+    <s v="Tower 3"/>
+    <s v="TBD - Humboldt"/>
     <x v="5"/>
     <s v="West Coast"/>
     <n v="2023"/>
@@ -3230,8 +3276,8 @@
   </r>
   <r>
     <s v="Monopile"/>
-    <x v="13"/>
-    <x v="10"/>
+    <s v="EEW"/>
+    <s v="Port of Paulsboro"/>
     <x v="2"/>
     <s v="Central Atlantic"/>
     <n v="2020"/>
@@ -3243,8 +3289,8 @@
   </r>
   <r>
     <m/>
-    <x v="14"/>
-    <x v="8"/>
+    <s v="US Wind"/>
+    <s v="Tradepoint Atlantic"/>
     <x v="2"/>
     <s v="South Atlantic"/>
     <n v="2021"/>
@@ -3256,8 +3302,8 @@
   </r>
   <r>
     <s v="Jacket"/>
-    <x v="15"/>
-    <x v="11"/>
+    <s v="Jacket 1"/>
+    <s v="Port of New Orleans"/>
     <x v="9"/>
     <s v="Gulf of Mexico"/>
     <n v="2023"/>
@@ -3269,8 +3315,8 @@
   </r>
   <r>
     <s v="GBF"/>
-    <x v="16"/>
-    <x v="12"/>
+    <s v="GBF 1"/>
+    <s v="Radio Island, Morehead City"/>
     <x v="1"/>
     <s v="South Atlantic"/>
     <n v="2025"/>
@@ -3282,8 +3328,8 @@
   </r>
   <r>
     <s v="Transition piece"/>
-    <x v="17"/>
-    <x v="7"/>
+    <s v="Smulders"/>
+    <s v="Port of Albany"/>
     <x v="6"/>
     <s v="Central Atlantic"/>
     <n v="2021"/>
@@ -3295,8 +3341,8 @@
   </r>
   <r>
     <m/>
-    <x v="18"/>
-    <x v="13"/>
+    <s v="Transition piece 1"/>
+    <s v="Port of Coeymans"/>
     <x v="6"/>
     <s v="Central Atlantic"/>
     <n v="2023"/>
@@ -3308,8 +3354,8 @@
   </r>
   <r>
     <s v="Array cable"/>
-    <x v="19"/>
-    <x v="8"/>
+    <s v="Hellenic"/>
+    <s v="Tradepoint Atlantic"/>
     <x v="7"/>
     <s v="South Atlantic"/>
     <n v="2021"/>
@@ -3321,8 +3367,8 @@
   </r>
   <r>
     <m/>
-    <x v="20"/>
-    <x v="14"/>
+    <s v="Array cable 1"/>
+    <s v="Arthur Kill Terminal"/>
     <x v="6"/>
     <s v="Central Atlantic"/>
     <n v="2023"/>
@@ -3334,8 +3380,8 @@
   </r>
   <r>
     <m/>
-    <x v="21"/>
-    <x v="15"/>
+    <s v="Array cable 2"/>
+    <s v="Mystic River, Everett"/>
     <x v="10"/>
     <s v="North Atlantic"/>
     <n v="2023"/>
@@ -3347,8 +3393,8 @@
   </r>
   <r>
     <s v="Export cable"/>
-    <x v="22"/>
-    <x v="16"/>
+    <s v="Nexans"/>
+    <s v="Goose Island"/>
     <x v="11"/>
     <s v="South Atlantic"/>
     <n v="2018"/>
@@ -3360,8 +3406,8 @@
   </r>
   <r>
     <m/>
-    <x v="23"/>
-    <x v="17"/>
+    <s v="Prysmian"/>
+    <s v="Brayton Point"/>
     <x v="10"/>
     <s v="North Atlantic"/>
     <n v="2021"/>
@@ -3373,8 +3419,8 @@
   </r>
   <r>
     <m/>
-    <x v="24"/>
-    <x v="18"/>
+    <s v="Export cable 1"/>
+    <s v="Quonset Business Park / Port of Davisville"/>
     <x v="4"/>
     <s v="North Atlantic"/>
     <n v="2023"/>
@@ -3386,8 +3432,8 @@
   </r>
   <r>
     <m/>
-    <x v="25"/>
-    <x v="19"/>
+    <s v="Export cable 2"/>
+    <s v="Columbus Terminal"/>
     <x v="11"/>
     <s v="South Atlantic"/>
     <n v="2023"/>
@@ -3399,8 +3445,8 @@
   </r>
   <r>
     <s v="Steel plates"/>
-    <x v="26"/>
-    <x v="20"/>
+    <s v="Nucor"/>
+    <s v="Brandenburg "/>
     <x v="12"/>
     <s v="South Atlantic"/>
     <n v="2021"/>
@@ -3412,8 +3458,8 @@
   </r>
   <r>
     <m/>
-    <x v="27"/>
-    <x v="21"/>
+    <s v="Steel plate 1"/>
+    <s v="Port of Brunswick"/>
     <x v="13"/>
     <s v="South Atlantic"/>
     <n v="2023"/>
@@ -3425,8 +3471,8 @@
   </r>
   <r>
     <s v="Casting"/>
-    <x v="28"/>
-    <x v="22"/>
+    <s v="Casting 1"/>
+    <m/>
     <x v="14"/>
     <s v="Other"/>
     <n v="2023"/>
@@ -3438,8 +3484,8 @@
   </r>
   <r>
     <s v="Flange"/>
-    <x v="29"/>
-    <x v="23"/>
+    <s v="Flange 1"/>
+    <s v="Schiller Newington, Portsmouth"/>
     <x v="15"/>
     <s v="North Atlantic"/>
     <n v="2023"/>
@@ -3451,8 +3497,8 @@
   </r>
   <r>
     <s v="Semisubmersible"/>
-    <x v="30"/>
-    <x v="6"/>
+    <s v="Semisubmersible 1"/>
+    <s v="TBD - Humboldt"/>
     <x v="5"/>
     <s v="West Coast"/>
     <n v="2024"/>
@@ -3464,8 +3510,8 @@
   </r>
   <r>
     <m/>
-    <x v="31"/>
-    <x v="24"/>
+    <s v="Semisubmersible 2"/>
+    <s v="TBD - Central Coast"/>
     <x v="5"/>
     <s v="West Coast"/>
     <n v="2025"/>
@@ -3477,8 +3523,8 @@
   </r>
   <r>
     <m/>
-    <x v="32"/>
-    <x v="4"/>
+    <s v="Semisubmersible 3"/>
+    <s v="TBD - Coos Bay"/>
     <x v="3"/>
     <s v="West Coast"/>
     <n v="2026"/>
@@ -3489,9 +3535,35 @@
     <n v="4"/>
   </r>
   <r>
-    <s v="Stationkeeping"/>
-    <x v="33"/>
-    <x v="25"/>
+    <m/>
+    <s v="Semisubmersible 4"/>
+    <s v="Port of New Orleans"/>
+    <x v="9"/>
+    <s v="Gulf of Mexico"/>
+    <n v="2031"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="0.25"/>
+    <n v="2033"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <m/>
+    <s v="Semisubmersible 5"/>
+    <s v="Portsmouth Marine Terminal"/>
+    <x v="0"/>
+    <s v="South Atlantic"/>
+    <n v="2030"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="0.25"/>
+    <n v="2032"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <m/>
+    <s v="Semisubmersible 6"/>
+    <s v="TBD - WA"/>
     <x v="16"/>
     <s v="West Coast"/>
     <n v="2024"/>
@@ -3503,10 +3575,36 @@
   </r>
   <r>
     <m/>
-    <x v="34"/>
-    <x v="25"/>
-    <x v="16"/>
-    <s v="West Coast"/>
+    <s v="Semisubmersible 7"/>
+    <s v="TBD - TX"/>
+    <x v="17"/>
+    <s v="Gulf of Mexico"/>
+    <n v="2028"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="0.25"/>
+    <n v="2031"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <s v="Stationkeeping"/>
+    <s v="Mooring chain 1"/>
+    <s v="TBD - TX"/>
+    <x v="17"/>
+    <s v="Gulf of Mexico"/>
+    <n v="2024"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="0.25"/>
+    <n v="2028"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <m/>
+    <s v="Mooring rope 1"/>
+    <s v="TBD - LA"/>
+    <x v="9"/>
+    <s v="Gulf of Mexico"/>
     <n v="2024"/>
     <n v="3"/>
     <n v="2"/>
@@ -3518,83 +3616,14 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5CA5F775-FB12-4A7B-98B7-3842EC7091C4}" name="PivotTable1" cacheId="17" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
-  <location ref="G48:H66" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5CA5F775-FB12-4A7B-98B7-3842EC7091C4}" name="PivotTable1" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
+  <location ref="H51:I70" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0">
-      <items count="36">
-        <item x="20"/>
-        <item x="21"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="28"/>
-        <item x="13"/>
-        <item x="24"/>
-        <item x="25"/>
-        <item x="29"/>
-        <item x="16"/>
-        <item x="5"/>
-        <item x="19"/>
-        <item x="15"/>
-        <item x="9"/>
-        <item x="33"/>
-        <item x="34"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="22"/>
-        <item x="26"/>
-        <item x="23"/>
-        <item x="30"/>
-        <item x="31"/>
-        <item x="32"/>
-        <item x="0"/>
-        <item x="17"/>
-        <item x="27"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="18"/>
-        <item x="14"/>
-        <item x="6"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="27">
-        <item x="14"/>
-        <item x="20"/>
-        <item x="17"/>
-        <item x="19"/>
-        <item x="1"/>
-        <item x="16"/>
-        <item x="15"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item x="7"/>
-        <item x="21"/>
-        <item x="13"/>
-        <item x="11"/>
-        <item x="10"/>
-        <item x="0"/>
-        <item x="18"/>
-        <item x="12"/>
-        <item x="23"/>
-        <item x="9"/>
-        <item x="5"/>
-        <item x="24"/>
-        <item x="4"/>
-        <item x="6"/>
-        <item x="25"/>
-        <item x="8"/>
-        <item x="22"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
-      <items count="18">
+      <items count="19">
         <item x="5"/>
         <item x="13"/>
         <item x="12"/>
@@ -3612,6 +3641,7 @@
         <item x="11"/>
         <item x="0"/>
         <item x="16"/>
+        <item x="17"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -3626,7 +3656,7 @@
   <rowFields count="1">
     <field x="3"/>
   </rowFields>
-  <rowItems count="18">
+  <rowItems count="19">
     <i>
       <x/>
     </i>
@@ -3677,6 +3707,9 @@
     </i>
     <i>
       <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
     </i>
     <i t="grand">
       <x/>
@@ -3996,1618 +4029,1863 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F1FF48-4396-4FE3-ABD9-234FB66F60F4}">
-  <dimension ref="A1:L66"/>
+  <dimension ref="A1:M70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L57" sqref="L57"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" customWidth="1"/>
-    <col min="3" max="3" width="42.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="82.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="25.140625" customWidth="1"/>
+    <col min="4" max="4" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="82.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="D3">
+        <v>0.25</v>
+      </c>
+      <c r="E3" t="s">
         <v>95</v>
       </c>
-      <c r="B3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C3">
-        <v>0.25</v>
-      </c>
-      <c r="D3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4">
+        <v>34</v>
+      </c>
+      <c r="D4">
         <v>2023</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-      <c r="D5" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L7" s="1"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="L8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="M8" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="L8" s="1" t="s">
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
         <v>42</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
+        <v>151</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9">
+        <v>2021</v>
+      </c>
+      <c r="H9">
+        <f>$D$5</f>
+        <v>3</v>
+      </c>
+      <c r="I9">
+        <v>3</v>
+      </c>
+      <c r="J9">
+        <f>$D$3</f>
+        <v>0.25</v>
+      </c>
+      <c r="K9">
+        <f>ROUNDDOWN(G9+H9+I9*(1-J9),0)</f>
+        <v>2026</v>
+      </c>
+      <c r="L9">
+        <f>K9-G9</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>43</v>
       </c>
-      <c r="C9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="C10" t="s">
+        <v>152</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" t="s">
         <v>5</v>
       </c>
-      <c r="F9">
-        <v>2021</v>
-      </c>
-      <c r="G9">
-        <f>$C$5</f>
+      <c r="G10">
+        <v>2023</v>
+      </c>
+      <c r="H10">
+        <f>$D$5</f>
         <v>3</v>
       </c>
-      <c r="H9">
+      <c r="I10">
         <v>3</v>
       </c>
-      <c r="I9">
-        <f>$C$3</f>
+      <c r="J10">
+        <f t="shared" ref="J10:J13" si="0">$D$3</f>
         <v>0.25</v>
       </c>
-      <c r="J9">
-        <f>ROUNDDOWN(F9+G9+H9*(1-I9),0)</f>
-        <v>2026</v>
-      </c>
-      <c r="K9">
-        <f>J9-F9</f>
+      <c r="K10">
+        <f>ROUNDDOWN(G10+H10+I10*(1-J10),0)</f>
+        <v>2028</v>
+      </c>
+      <c r="L10">
+        <f t="shared" ref="L10:L46" si="1">K10-G10</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="M10" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" t="s">
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" t="s">
+        <v>148</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11">
+        <v>2023</v>
+      </c>
+      <c r="H11">
+        <f>$D$5</f>
+        <v>3</v>
+      </c>
+      <c r="I11">
+        <v>3</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="K11">
+        <f t="shared" ref="K11:K46" si="2">ROUNDDOWN(G11+H11+I11*(1-J11),0)</f>
+        <v>2028</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="F10">
+      <c r="M11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" t="s">
+        <v>150</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12">
         <v>2023</v>
       </c>
-      <c r="G10">
-        <f t="shared" ref="G10:G36" si="0">$C$5</f>
+      <c r="H12">
+        <f>$D$5</f>
         <v>3</v>
       </c>
-      <c r="H10">
+      <c r="I12">
         <v>3</v>
       </c>
-      <c r="I10">
-        <f t="shared" ref="I10:I13" si="1">$C$3</f>
+      <c r="J12">
+        <f t="shared" si="0"/>
         <v>0.25</v>
-      </c>
-      <c r="J10">
-        <f>ROUNDDOWN(F10+G10+H10*(1-I10),0)</f>
-        <v>2028</v>
-      </c>
-      <c r="K10">
-        <f t="shared" ref="K10:K43" si="2">J10-F10</f>
-        <v>5</v>
-      </c>
-      <c r="L10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" t="s">
-        <v>5</v>
-      </c>
-      <c r="F11">
-        <v>2023</v>
-      </c>
-      <c r="G11">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="H11">
-        <v>3</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="1"/>
-        <v>0.25</v>
-      </c>
-      <c r="J11">
-        <f t="shared" ref="J11:J43" si="3">ROUNDDOWN(F11+G11+H11*(1-I11),0)</f>
-        <v>2028</v>
-      </c>
-      <c r="K11">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="L11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D12" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F12">
-        <v>2023</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="H12">
-        <v>3</v>
-      </c>
-      <c r="I12">
-        <f t="shared" si="1"/>
-        <v>0.25</v>
-      </c>
-      <c r="J12">
-        <f t="shared" si="3"/>
-        <v>2028</v>
       </c>
       <c r="K12">
         <f t="shared" si="2"/>
+        <v>2028</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="L12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>123</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D13" t="s">
-        <v>127</v>
+        <v>121</v>
+      </c>
+      <c r="C13" t="s">
+        <v>149</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>129</v>
       </c>
       <c r="E13" t="s">
-        <v>128</v>
-      </c>
-      <c r="F13">
+        <v>125</v>
+      </c>
+      <c r="F13" t="s">
+        <v>126</v>
+      </c>
+      <c r="G13">
         <v>2024</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>4</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>3</v>
       </c>
-      <c r="I13">
-        <f t="shared" si="1"/>
+      <c r="J13">
+        <f t="shared" si="0"/>
         <v>0.25</v>
-      </c>
-      <c r="J13">
-        <f t="shared" si="3"/>
-        <v>2030</v>
       </c>
       <c r="K13">
         <f t="shared" si="2"/>
+        <v>2030</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" t="s">
         <v>50</v>
       </c>
-      <c r="B14" t="s">
-        <v>51</v>
-      </c>
       <c r="C14" t="s">
-        <v>48</v>
+        <v>150</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="E14" t="s">
-        <v>25</v>
-      </c>
-      <c r="F14">
+        <v>26</v>
+      </c>
+      <c r="F14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14">
         <v>2021</v>
       </c>
-      <c r="G14">
-        <f t="shared" si="0"/>
+      <c r="H14">
+        <f>$D$5</f>
         <v>3</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>3</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <f>1/3</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="J14">
-        <f t="shared" si="3"/>
-        <v>2026</v>
-      </c>
       <c r="K14">
         <f t="shared" si="2"/>
+        <v>2026</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="L14" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C15" t="s">
-        <v>48</v>
+        <v>150</v>
       </c>
       <c r="D15" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="E15" t="s">
-        <v>25</v>
-      </c>
-      <c r="F15">
+        <v>26</v>
+      </c>
+      <c r="F15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15">
         <v>2021</v>
       </c>
-      <c r="G15">
-        <f t="shared" si="0"/>
+      <c r="H15">
+        <f>$D$5</f>
         <v>3</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>3</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <f>1/3</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="J15">
-        <f t="shared" si="3"/>
-        <v>2026</v>
-      </c>
       <c r="K15">
         <f t="shared" si="2"/>
+        <v>2026</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="L15" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M15" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" t="s">
-        <v>18</v>
+        <v>52</v>
+      </c>
+      <c r="C16" t="s">
+        <v>153</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="E16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F16">
+        <v>17</v>
+      </c>
+      <c r="F16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16">
         <v>2023</v>
       </c>
-      <c r="G16">
-        <f t="shared" si="0"/>
+      <c r="H16">
+        <f>$D$5</f>
         <v>3</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>3</v>
       </c>
-      <c r="I16">
-        <f t="shared" ref="I16" si="4">$C$3</f>
+      <c r="J16">
+        <f t="shared" ref="J16" si="3">$D$3</f>
         <v>0.25</v>
-      </c>
-      <c r="J16">
-        <f t="shared" si="3"/>
-        <v>2028</v>
       </c>
       <c r="K16">
         <f t="shared" si="2"/>
+        <v>2028</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>125</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="D17" t="s">
-        <v>124</v>
+        <v>123</v>
+      </c>
+      <c r="C17" t="s">
+        <v>154</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="E17" t="s">
-        <v>128</v>
-      </c>
-      <c r="F17">
+        <v>122</v>
+      </c>
+      <c r="F17" t="s">
+        <v>126</v>
+      </c>
+      <c r="G17">
         <v>2023</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>4</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>3</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>0.25</v>
       </c>
-      <c r="J17">
-        <f t="shared" ref="J17" si="5">ROUNDDOWN(F17+G17+H17*(1-I17),0)</f>
+      <c r="K17">
+        <f t="shared" ref="K17" si="4">ROUNDDOWN(G17+H17+I17*(1-J17),0)</f>
         <v>2029</v>
       </c>
-      <c r="K17">
-        <f t="shared" ref="K17" si="6">J17-F17</f>
+      <c r="L17">
+        <f t="shared" ref="L17" si="5">K17-G17</f>
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" t="s">
         <v>54</v>
       </c>
-      <c r="B18" t="s">
-        <v>55</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="C18" t="s">
+        <v>155</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" t="s">
         <v>24</v>
       </c>
-      <c r="E18" t="s">
-        <v>25</v>
-      </c>
-      <c r="F18">
+      <c r="G18">
         <v>2021</v>
       </c>
-      <c r="G18">
-        <f t="shared" si="0"/>
+      <c r="H18">
+        <f>$D$5</f>
         <v>3</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>2.5</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>0.8</v>
-      </c>
-      <c r="J18">
-        <f t="shared" si="3"/>
-        <v>2024</v>
       </c>
       <c r="K18">
         <f t="shared" si="2"/>
+        <v>2024</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="L18" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M18" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" t="s">
+        <v>156</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>6</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>5</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>2023</v>
       </c>
-      <c r="G19">
-        <f t="shared" si="0"/>
+      <c r="H19">
+        <f>$D$5</f>
         <v>3</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <v>2.5</v>
       </c>
-      <c r="I19">
-        <f t="shared" ref="I19:I21" si="7">$C$3</f>
+      <c r="J19">
+        <f t="shared" ref="J19:J21" si="6">$D$3</f>
         <v>0.25</v>
-      </c>
-      <c r="J19">
-        <f t="shared" si="3"/>
-        <v>2027</v>
       </c>
       <c r="K19">
         <f t="shared" si="2"/>
+        <v>2027</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="L19" t="s">
+      <c r="M19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>60</v>
-      </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" t="s">
+        <v>157</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" t="s">
         <v>19</v>
       </c>
-      <c r="D20" t="s">
-        <v>20</v>
-      </c>
-      <c r="E20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F20">
+      <c r="F20" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20">
         <v>2023</v>
       </c>
-      <c r="G20">
-        <f t="shared" si="0"/>
+      <c r="H20">
+        <f>$D$5</f>
         <v>3</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <v>2.5</v>
       </c>
-      <c r="I20">
-        <f t="shared" si="7"/>
+      <c r="J20">
+        <f t="shared" si="6"/>
         <v>0.25</v>
-      </c>
-      <c r="J20">
-        <f t="shared" si="3"/>
-        <v>2027</v>
       </c>
       <c r="K20">
         <f t="shared" si="2"/>
+        <v>2027</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="L20" t="s">
+      <c r="M20" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>124</v>
+      </c>
+      <c r="C21" t="s">
+        <v>154</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E21" t="s">
+        <v>122</v>
+      </c>
+      <c r="F21" t="s">
+        <v>126</v>
+      </c>
+      <c r="G21">
+        <v>2023</v>
+      </c>
+      <c r="H21">
+        <v>4</v>
+      </c>
+      <c r="I21">
+        <v>2.5</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="6"/>
+        <v>0.25</v>
+      </c>
+      <c r="K21">
+        <f t="shared" ref="K21" si="7">ROUNDDOWN(G21+H21+I21*(1-J21),0)</f>
+        <v>2028</v>
+      </c>
+      <c r="L21">
+        <f t="shared" ref="L21" si="8">K21-G21</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>126</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="D21" t="s">
-        <v>124</v>
-      </c>
-      <c r="E21" t="s">
-        <v>128</v>
-      </c>
-      <c r="F21">
-        <v>2023</v>
-      </c>
-      <c r="G21">
-        <v>4</v>
-      </c>
-      <c r="H21">
-        <v>2.5</v>
-      </c>
-      <c r="I21">
-        <f t="shared" si="7"/>
-        <v>0.25</v>
-      </c>
-      <c r="J21">
-        <f t="shared" ref="J21" si="8">ROUNDDOWN(F21+G21+H21*(1-I21),0)</f>
-        <v>2028</v>
-      </c>
-      <c r="K21">
-        <f t="shared" ref="K21" si="9">J21-F21</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="B22" t="s">
         <v>62</v>
       </c>
-      <c r="B22" t="s">
-        <v>63</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="C22" t="s">
+        <v>158</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>27</v>
       </c>
       <c r="E22" t="s">
-        <v>25</v>
-      </c>
-      <c r="F22">
+        <v>26</v>
+      </c>
+      <c r="F22" t="s">
+        <v>24</v>
+      </c>
+      <c r="G22">
         <v>2020</v>
       </c>
-      <c r="G22">
-        <f t="shared" si="0"/>
+      <c r="H22">
+        <f>$D$5</f>
         <v>3</v>
       </c>
-      <c r="H22">
+      <c r="I22">
         <v>2</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <v>0.5</v>
-      </c>
-      <c r="J22">
-        <f t="shared" si="3"/>
-        <v>2024</v>
       </c>
       <c r="K22">
         <f t="shared" si="2"/>
+        <v>2024</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="L22" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M22" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>64</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D23" t="s">
-        <v>27</v>
+        <v>63</v>
+      </c>
+      <c r="C23" t="s">
+        <v>156</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="E23" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23" t="s">
         <v>5</v>
       </c>
-      <c r="F23">
+      <c r="G23">
         <v>2021</v>
       </c>
-      <c r="G23">
-        <f t="shared" si="0"/>
+      <c r="H23">
+        <f>$D$5</f>
         <v>3</v>
       </c>
-      <c r="H23">
+      <c r="I23">
         <v>3.5</v>
       </c>
-      <c r="I23">
-        <f t="shared" ref="I23:I24" si="10">$C$3</f>
+      <c r="J23">
+        <f t="shared" ref="J23:J24" si="9">$D$3</f>
         <v>0.25</v>
-      </c>
-      <c r="J23">
-        <f t="shared" si="3"/>
-        <v>2026</v>
       </c>
       <c r="K23">
         <f t="shared" si="2"/>
+        <v>2026</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="L23" t="s">
+      <c r="M23" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="B24" t="s">
         <v>66</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
+        <v>159</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" t="s">
+        <v>22</v>
+      </c>
+      <c r="F24" t="s">
         <v>67</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="G24">
+        <v>2023</v>
+      </c>
+      <c r="H24">
+        <f>$D$5</f>
+        <v>3</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="9"/>
+        <v>0.25</v>
+      </c>
+      <c r="K24">
+        <f>ROUNDDOWN(G24+H24+I24*(1-J24),0)</f>
+        <v>2026</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="M24" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>105</v>
+      </c>
+      <c r="B25" t="s">
+        <v>106</v>
+      </c>
+      <c r="C25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" t="s">
+        <v>5</v>
+      </c>
+      <c r="G25">
+        <v>2025</v>
+      </c>
+      <c r="H25">
+        <v>2</v>
+      </c>
+      <c r="I25">
+        <v>1</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <f>ROUNDDOWN(G25+H25+I25*(1-J25),0)</f>
+        <v>2028</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="M25" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" t="s">
+        <v>155</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E26" t="s">
         <v>23</v>
       </c>
-      <c r="E24" t="s">
-        <v>68</v>
-      </c>
-      <c r="F24">
+      <c r="F26" t="s">
+        <v>24</v>
+      </c>
+      <c r="G26">
+        <v>2021</v>
+      </c>
+      <c r="H26">
+        <f>$D$5</f>
+        <v>3</v>
+      </c>
+      <c r="I26">
+        <v>2.5</v>
+      </c>
+      <c r="J26">
+        <v>0.25</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="2"/>
+        <v>2025</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="M26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>108</v>
+      </c>
+      <c r="C27" t="s">
+        <v>161</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E27" t="s">
+        <v>23</v>
+      </c>
+      <c r="F27" t="s">
+        <v>24</v>
+      </c>
+      <c r="G27">
         <v>2023</v>
       </c>
-      <c r="G24">
-        <f t="shared" si="0"/>
+      <c r="H27">
+        <f>$D$5</f>
         <v>3</v>
       </c>
-      <c r="H24">
-        <v>1</v>
-      </c>
-      <c r="I24">
+      <c r="I27">
+        <v>2.5</v>
+      </c>
+      <c r="J27">
+        <f t="shared" ref="J27:J29" si="10">$D$3</f>
+        <v>0.25</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="2"/>
+        <v>2027</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="M27" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28" t="s">
+        <v>156</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E28" t="s">
+        <v>6</v>
+      </c>
+      <c r="F28" t="s">
+        <v>5</v>
+      </c>
+      <c r="G28">
+        <v>2021</v>
+      </c>
+      <c r="H28">
+        <f>$D$5</f>
+        <v>3</v>
+      </c>
+      <c r="I28">
+        <v>5</v>
+      </c>
+      <c r="J28">
         <f t="shared" si="10"/>
         <v>0.25</v>
       </c>
-      <c r="J24">
-        <f>ROUNDDOWN(F24+G24+H24*(1-I24),0)</f>
-        <v>2026</v>
-      </c>
-      <c r="K24">
+      <c r="K28">
         <f t="shared" si="2"/>
+        <v>2027</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>75</v>
+      </c>
+      <c r="C29" t="s">
+        <v>162</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E29" t="s">
+        <v>23</v>
+      </c>
+      <c r="F29" t="s">
+        <v>24</v>
+      </c>
+      <c r="G29">
+        <v>2023</v>
+      </c>
+      <c r="H29">
+        <f>$D$5</f>
         <v>3</v>
       </c>
-      <c r="L24" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>107</v>
-      </c>
-      <c r="B25" t="s">
-        <v>108</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D25" t="s">
-        <v>10</v>
-      </c>
-      <c r="E25" t="s">
+      <c r="I29">
         <v>5</v>
       </c>
-      <c r="F25">
-        <v>2025</v>
-      </c>
-      <c r="G25">
+      <c r="J29">
+        <f t="shared" si="10"/>
+        <v>0.25</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="2"/>
+        <v>2029</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="M29" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30" t="s">
+        <v>163</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E30" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" t="s">
+        <v>5</v>
+      </c>
+      <c r="G30">
+        <v>2018</v>
+      </c>
+      <c r="H30">
+        <f>$D$5</f>
+        <v>3</v>
+      </c>
+      <c r="I30" t="s">
+        <v>80</v>
+      </c>
+      <c r="J30" t="s">
+        <v>80</v>
+      </c>
+      <c r="K30">
+        <v>2020</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="H25">
-        <v>1</v>
-      </c>
-      <c r="I25">
-        <v>0</v>
-      </c>
-      <c r="J25">
-        <f>ROUNDDOWN(F25+G25+H25*(1-I25),0)</f>
-        <v>2028</v>
-      </c>
-      <c r="K25">
+      <c r="M30" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>82</v>
+      </c>
+      <c r="C31" t="s">
+        <v>164</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E31" t="s">
+        <v>14</v>
+      </c>
+      <c r="F31" t="s">
+        <v>15</v>
+      </c>
+      <c r="G31">
+        <v>2021</v>
+      </c>
+      <c r="H31">
+        <f>$D$5</f>
+        <v>3</v>
+      </c>
+      <c r="I31">
+        <v>5</v>
+      </c>
+      <c r="J31">
+        <f t="shared" ref="J31:J35" si="11">$D$3</f>
+        <v>0.25</v>
+      </c>
+      <c r="K31">
         <f t="shared" si="2"/>
+        <v>2027</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>83</v>
+      </c>
+      <c r="C32" t="s">
+        <v>165</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E32" t="s">
+        <v>17</v>
+      </c>
+      <c r="F32" t="s">
+        <v>15</v>
+      </c>
+      <c r="G32">
+        <v>2023</v>
+      </c>
+      <c r="H32">
+        <f>$D$5</f>
         <v>3</v>
       </c>
-      <c r="L25" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>70</v>
-      </c>
-      <c r="B26" t="s">
-        <v>71</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D26" t="s">
-        <v>24</v>
-      </c>
-      <c r="E26" t="s">
-        <v>25</v>
-      </c>
-      <c r="F26">
-        <v>2021</v>
-      </c>
-      <c r="G26">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="H26">
-        <v>2.5</v>
-      </c>
-      <c r="I26">
-        <v>0.25</v>
-      </c>
-      <c r="J26">
-        <f t="shared" si="3"/>
-        <v>2025</v>
-      </c>
-      <c r="K26">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="L26" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>110</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D27" t="s">
-        <v>24</v>
-      </c>
-      <c r="E27" t="s">
-        <v>25</v>
-      </c>
-      <c r="F27">
-        <v>2023</v>
-      </c>
-      <c r="G27">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="H27">
-        <v>2.5</v>
-      </c>
-      <c r="I27">
-        <f t="shared" ref="I27:I29" si="11">$C$3</f>
-        <v>0.25</v>
-      </c>
-      <c r="J27">
-        <f t="shared" si="3"/>
-        <v>2027</v>
-      </c>
-      <c r="K27">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="L27" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>74</v>
-      </c>
-      <c r="B28" t="s">
-        <v>75</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D28" t="s">
-        <v>6</v>
-      </c>
-      <c r="E28" t="s">
+      <c r="I32">
         <v>5</v>
       </c>
-      <c r="F28">
-        <v>2021</v>
-      </c>
-      <c r="G28">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="H28">
-        <v>5</v>
-      </c>
-      <c r="I28">
+      <c r="J32">
         <f t="shared" si="11"/>
         <v>0.25</v>
       </c>
-      <c r="J28">
-        <f t="shared" si="3"/>
-        <v>2027</v>
-      </c>
-      <c r="K28">
+      <c r="K32">
         <f t="shared" si="2"/>
+        <v>2029</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>76</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D29" t="s">
-        <v>24</v>
-      </c>
-      <c r="E29" t="s">
-        <v>25</v>
-      </c>
-      <c r="F29">
+      <c r="M32" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>85</v>
+      </c>
+      <c r="C33" t="s">
+        <v>166</v>
+      </c>
+      <c r="D33" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33" t="s">
+        <v>5</v>
+      </c>
+      <c r="G33">
         <v>2023</v>
       </c>
-      <c r="G29">
-        <f t="shared" si="0"/>
+      <c r="H33">
+        <f>$D$5</f>
         <v>3</v>
       </c>
-      <c r="H29">
+      <c r="I33">
         <v>5</v>
       </c>
-      <c r="I29">
+      <c r="J33">
         <f t="shared" si="11"/>
         <v>0.25</v>
       </c>
-      <c r="J29">
-        <f t="shared" si="3"/>
-        <v>2029</v>
-      </c>
-      <c r="K29">
-        <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-      <c r="L29" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>78</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D30" t="s">
-        <v>15</v>
-      </c>
-      <c r="E30" t="s">
-        <v>16</v>
-      </c>
-      <c r="F30">
-        <v>2023</v>
-      </c>
-      <c r="G30">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="H30">
-        <v>5</v>
-      </c>
-      <c r="I30">
-        <f t="shared" ref="I30" si="12">$C$3</f>
-        <v>0.25</v>
-      </c>
-      <c r="J30">
-        <f t="shared" si="3"/>
-        <v>2029</v>
-      </c>
-      <c r="K30">
-        <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>79</v>
-      </c>
-      <c r="B31" t="s">
-        <v>80</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D31" t="s">
-        <v>13</v>
-      </c>
-      <c r="E31" t="s">
-        <v>5</v>
-      </c>
-      <c r="F31">
-        <v>2018</v>
-      </c>
-      <c r="G31">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="H31" t="s">
-        <v>82</v>
-      </c>
-      <c r="I31" t="s">
-        <v>82</v>
-      </c>
-      <c r="J31">
-        <v>2020</v>
-      </c>
-      <c r="K31">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="L31" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>84</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D32" t="s">
-        <v>15</v>
-      </c>
-      <c r="E32" t="s">
-        <v>16</v>
-      </c>
-      <c r="F32">
-        <v>2021</v>
-      </c>
-      <c r="G32">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="H32">
-        <v>5</v>
-      </c>
-      <c r="I32">
-        <f t="shared" ref="I32:I36" si="13">$C$3</f>
-        <v>0.25</v>
-      </c>
-      <c r="J32">
-        <f t="shared" si="3"/>
-        <v>2027</v>
-      </c>
-      <c r="K32">
-        <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>85</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D33" t="s">
-        <v>18</v>
-      </c>
-      <c r="E33" t="s">
-        <v>16</v>
-      </c>
-      <c r="F33">
-        <v>2023</v>
-      </c>
-      <c r="G33">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="H33">
-        <v>5</v>
-      </c>
-      <c r="I33">
-        <f t="shared" si="13"/>
-        <v>0.25</v>
-      </c>
-      <c r="J33">
-        <f t="shared" si="3"/>
-        <v>2029</v>
-      </c>
       <c r="K33">
         <f t="shared" si="2"/>
+        <v>2029</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="L33" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>87</v>
+      </c>
       <c r="B34" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C34" t="s">
-        <v>12</v>
-      </c>
-      <c r="D34" t="s">
-        <v>13</v>
+        <v>167</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>89</v>
       </c>
       <c r="E34" t="s">
+        <v>90</v>
+      </c>
+      <c r="F34" t="s">
         <v>5</v>
       </c>
-      <c r="F34">
-        <v>2023</v>
-      </c>
       <c r="G34">
-        <f t="shared" si="0"/>
+        <v>2021</v>
+      </c>
+      <c r="H34">
+        <f>$D$5</f>
         <v>3</v>
       </c>
-      <c r="H34">
-        <v>5</v>
-      </c>
       <c r="I34">
-        <f t="shared" si="13"/>
+        <v>2</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="11"/>
         <v>0.25</v>
-      </c>
-      <c r="J34">
-        <f t="shared" si="3"/>
-        <v>2029</v>
       </c>
       <c r="K34">
         <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>89</v>
-      </c>
+        <v>2025</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>90</v>
-      </c>
-      <c r="C35" s="2" t="s">
         <v>91</v>
       </c>
+      <c r="C35" t="s">
+        <v>168</v>
+      </c>
       <c r="D35" t="s">
-        <v>92</v>
+        <v>3</v>
       </c>
       <c r="E35" t="s">
+        <v>4</v>
+      </c>
+      <c r="F35" t="s">
         <v>5</v>
       </c>
-      <c r="F35">
-        <v>2021</v>
-      </c>
       <c r="G35">
-        <f t="shared" si="0"/>
+        <v>2023</v>
+      </c>
+      <c r="H35">
+        <f>$D$5</f>
         <v>3</v>
       </c>
-      <c r="H35">
-        <v>2</v>
-      </c>
       <c r="I35">
-        <f t="shared" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="11"/>
         <v>0.25</v>
-      </c>
-      <c r="J35">
-        <f t="shared" si="3"/>
-        <v>2025</v>
       </c>
       <c r="K35">
         <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2029</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>109</v>
+      </c>
       <c r="B36" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="C36" t="s">
-        <v>3</v>
-      </c>
-      <c r="D36" t="s">
-        <v>4</v>
+        <v>169</v>
       </c>
       <c r="E36" t="s">
-        <v>5</v>
-      </c>
-      <c r="F36">
+        <v>111</v>
+      </c>
+      <c r="F36" t="s">
+        <v>112</v>
+      </c>
+      <c r="G36">
         <v>2023</v>
       </c>
-      <c r="G36">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
       <c r="H36">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I36">
-        <f t="shared" si="13"/>
-        <v>0.25</v>
+        <v>2</v>
       </c>
       <c r="J36">
-        <f t="shared" si="3"/>
-        <v>2029</v>
+        <v>0</v>
       </c>
       <c r="K36">
         <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2025</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="M36" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>111</v>
+        <v>132</v>
       </c>
       <c r="B37" t="s">
-        <v>112</v>
+        <v>133</v>
+      </c>
+      <c r="C37" t="s">
+        <v>170</v>
       </c>
       <c r="D37" t="s">
-        <v>113</v>
+        <v>135</v>
       </c>
       <c r="E37" t="s">
-        <v>114</v>
-      </c>
-      <c r="F37">
+        <v>134</v>
+      </c>
+      <c r="F37" t="s">
+        <v>15</v>
+      </c>
+      <c r="G37">
         <v>2023</v>
       </c>
-      <c r="G37">
-        <v>0</v>
-      </c>
       <c r="H37">
+        <v>3</v>
+      </c>
+      <c r="I37">
         <v>2</v>
       </c>
-      <c r="I37">
-        <v>0</v>
-      </c>
       <c r="J37">
-        <f t="shared" si="3"/>
-        <v>2025</v>
+        <v>0.25</v>
       </c>
       <c r="K37">
         <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="L37" t="s">
+        <v>2027</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>114</v>
+      </c>
+      <c r="B38" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>135</v>
-      </c>
-      <c r="B38" t="s">
-        <v>136</v>
-      </c>
       <c r="C38" t="s">
-        <v>138</v>
+        <v>154</v>
       </c>
       <c r="D38" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="E38" t="s">
-        <v>16</v>
-      </c>
-      <c r="F38">
-        <v>2023</v>
+        <v>122</v>
+      </c>
+      <c r="F38" t="s">
+        <v>126</v>
       </c>
       <c r="G38">
-        <v>3</v>
+        <v>2024</v>
       </c>
       <c r="H38">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I38">
+        <v>1</v>
+      </c>
+      <c r="J38">
         <v>0.25</v>
-      </c>
-      <c r="J38">
-        <f t="shared" si="3"/>
-        <v>2027</v>
       </c>
       <c r="K38">
         <f t="shared" si="2"/>
+        <v>2028</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="M38" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
         <v>116</v>
       </c>
-      <c r="B39" t="s">
-        <v>117</v>
-      </c>
       <c r="C39" t="s">
-        <v>129</v>
+        <v>171</v>
       </c>
       <c r="D39" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="E39" t="s">
-        <v>128</v>
-      </c>
-      <c r="F39">
-        <v>2024</v>
+        <v>122</v>
+      </c>
+      <c r="F39" t="s">
+        <v>126</v>
       </c>
       <c r="G39">
+        <v>2025</v>
+      </c>
+      <c r="H39">
         <v>4</v>
       </c>
-      <c r="H39">
+      <c r="I39">
         <v>1</v>
       </c>
-      <c r="I39">
+      <c r="J39">
         <v>0.25</v>
-      </c>
-      <c r="J39">
-        <f t="shared" si="3"/>
-        <v>2028</v>
       </c>
       <c r="K39">
         <f t="shared" si="2"/>
+        <v>2029</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="L39" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M39" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C40" t="s">
-        <v>130</v>
+        <v>149</v>
       </c>
       <c r="D40" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="E40" t="s">
-        <v>128</v>
-      </c>
-      <c r="F40">
-        <v>2025</v>
+        <v>125</v>
+      </c>
+      <c r="F40" t="s">
+        <v>126</v>
       </c>
       <c r="G40">
+        <v>2026</v>
+      </c>
+      <c r="H40">
         <v>4</v>
       </c>
-      <c r="H40">
+      <c r="I40">
         <v>1</v>
       </c>
-      <c r="I40">
+      <c r="J40">
         <v>0.25</v>
-      </c>
-      <c r="J40">
-        <f t="shared" si="3"/>
-        <v>2029</v>
       </c>
       <c r="K40">
         <f t="shared" si="2"/>
+        <v>2030</v>
+      </c>
+      <c r="L40">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="L40" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M40" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>119</v>
+        <v>136</v>
       </c>
       <c r="C41" t="s">
-        <v>131</v>
+        <v>159</v>
       </c>
       <c r="D41" t="s">
-        <v>127</v>
+        <v>21</v>
       </c>
       <c r="E41" t="s">
-        <v>128</v>
-      </c>
-      <c r="F41">
-        <v>2026</v>
+        <v>22</v>
+      </c>
+      <c r="F41" t="s">
+        <v>67</v>
       </c>
       <c r="G41">
-        <v>4</v>
+        <v>2031</v>
       </c>
       <c r="H41">
+        <v>2</v>
+      </c>
+      <c r="I41">
         <v>1</v>
       </c>
-      <c r="I41">
+      <c r="J41">
         <v>0.25</v>
       </c>
-      <c r="J41">
-        <f t="shared" si="3"/>
+      <c r="K41">
+        <f t="shared" ref="K41:K42" si="12">ROUNDDOWN(G41+H41+I41*(1-J41),0)</f>
+        <v>2033</v>
+      </c>
+      <c r="L41">
+        <f t="shared" ref="L41:L42" si="13">K41-G41</f>
+        <v>2</v>
+      </c>
+      <c r="M41" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>139</v>
+      </c>
+      <c r="C42" t="s">
+        <v>151</v>
+      </c>
+      <c r="D42" t="s">
+        <v>7</v>
+      </c>
+      <c r="E42" t="s">
+        <v>8</v>
+      </c>
+      <c r="F42" t="s">
+        <v>5</v>
+      </c>
+      <c r="G42">
         <v>2030</v>
-      </c>
-      <c r="K41">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="L41" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>120</v>
-      </c>
-      <c r="B42" t="s">
-        <v>121</v>
-      </c>
-      <c r="C42" t="s">
-        <v>132</v>
-      </c>
-      <c r="D42" t="s">
-        <v>133</v>
-      </c>
-      <c r="E42" t="s">
-        <v>128</v>
-      </c>
-      <c r="F42">
-        <v>2024</v>
-      </c>
-      <c r="G42">
-        <v>3</v>
       </c>
       <c r="H42">
         <v>2</v>
       </c>
       <c r="I42">
+        <v>1</v>
+      </c>
+      <c r="J42">
         <v>0.25</v>
       </c>
-      <c r="J42">
-        <f t="shared" si="3"/>
+      <c r="K42">
+        <f t="shared" si="12"/>
+        <v>2032</v>
+      </c>
+      <c r="L42">
+        <f t="shared" si="13"/>
+        <v>2</v>
+      </c>
+      <c r="M42" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>144</v>
+      </c>
+      <c r="C43" t="s">
+        <v>172</v>
+      </c>
+      <c r="D43" t="s">
+        <v>130</v>
+      </c>
+      <c r="E43" t="s">
+        <v>131</v>
+      </c>
+      <c r="F43" t="s">
+        <v>126</v>
+      </c>
+      <c r="G43">
+        <v>2024</v>
+      </c>
+      <c r="H43">
+        <v>3</v>
+      </c>
+      <c r="I43">
+        <v>2</v>
+      </c>
+      <c r="J43">
+        <v>0.25</v>
+      </c>
+      <c r="K43">
+        <f t="shared" ref="K43:K44" si="14">ROUNDDOWN(G43+H43+I43*(1-J43),0)</f>
         <v>2028</v>
       </c>
-      <c r="K42">
+      <c r="L43">
+        <f t="shared" ref="L43:L44" si="15">K43-G43</f>
+        <v>4</v>
+      </c>
+      <c r="M43" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>145</v>
+      </c>
+      <c r="C44" t="s">
+        <v>173</v>
+      </c>
+      <c r="D44" t="s">
+        <v>140</v>
+      </c>
+      <c r="E44" t="s">
+        <v>141</v>
+      </c>
+      <c r="F44" t="s">
+        <v>67</v>
+      </c>
+      <c r="G44">
+        <v>2028</v>
+      </c>
+      <c r="H44">
+        <v>2</v>
+      </c>
+      <c r="I44">
+        <v>2</v>
+      </c>
+      <c r="J44">
+        <v>0.25</v>
+      </c>
+      <c r="K44">
+        <f t="shared" si="14"/>
+        <v>2031</v>
+      </c>
+      <c r="L44">
+        <f t="shared" si="15"/>
+        <v>3</v>
+      </c>
+      <c r="M44" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>118</v>
+      </c>
+      <c r="B45" t="s">
+        <v>119</v>
+      </c>
+      <c r="C45" t="s">
+        <v>174</v>
+      </c>
+      <c r="D45" t="s">
+        <v>140</v>
+      </c>
+      <c r="E45" t="s">
+        <v>141</v>
+      </c>
+      <c r="F45" t="s">
+        <v>67</v>
+      </c>
+      <c r="G45">
+        <v>2024</v>
+      </c>
+      <c r="H45">
+        <v>3</v>
+      </c>
+      <c r="I45">
+        <v>2</v>
+      </c>
+      <c r="J45">
+        <v>0.25</v>
+      </c>
+      <c r="K45">
         <f t="shared" si="2"/>
+        <v>2028</v>
+      </c>
+      <c r="L45">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
+      <c r="M45" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>120</v>
+      </c>
+      <c r="C46" t="s">
+        <v>175</v>
+      </c>
+      <c r="D46" t="s">
+        <v>143</v>
+      </c>
+      <c r="E46" t="s">
+        <v>22</v>
+      </c>
+      <c r="F46" t="s">
+        <v>67</v>
+      </c>
+      <c r="G46">
+        <v>2024</v>
+      </c>
+      <c r="H46">
+        <v>3</v>
+      </c>
+      <c r="I46">
+        <v>2</v>
+      </c>
+      <c r="J46">
+        <v>0.25</v>
+      </c>
+      <c r="K46">
+        <f t="shared" si="2"/>
+        <v>2028</v>
+      </c>
+      <c r="L46">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="M46" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H51" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="I51" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H52" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="C43" t="s">
-        <v>132</v>
-      </c>
-      <c r="D43" t="s">
-        <v>133</v>
-      </c>
-      <c r="E43" t="s">
-        <v>128</v>
-      </c>
-      <c r="F43">
-        <v>2024</v>
-      </c>
-      <c r="G43">
+      <c r="I52" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H53" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I53" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H54" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="I54" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H55" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I55" s="8">
         <v>3</v>
       </c>
-      <c r="H43">
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H56" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I56" s="8">
         <v>2</v>
       </c>
-      <c r="I43">
-        <v>0.25</v>
-      </c>
-      <c r="J43">
-        <f t="shared" si="3"/>
-        <v>2028</v>
-      </c>
-      <c r="K43">
-        <f t="shared" si="2"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H57" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I57" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H58" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I58" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H59" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I59" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H60" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="I60" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H61" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I61" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H62" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I62" s="8">
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H63" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="I63" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H64" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="I64" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H65" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I65" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H66" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I66" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H67" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I67" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H68" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="I68" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H69" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I69" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H70" s="7" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G48" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="H48" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="49" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G49" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="H49" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="50" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G50" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="H50" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G51" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="H51" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G52" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H52" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G53" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H53" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="54" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G54" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="H54" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="55" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G55" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H55" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G56" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="H56" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G57" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="H57" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G58" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H58" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="59" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G59" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H59" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="60" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G60" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="H60" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="61" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G61" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="H61" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G62" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H62" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="63" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G63" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H63" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="64" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G64" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H64" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="65" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G65" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="H65" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="66" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G66" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="H66" s="8">
-        <v>35</v>
+      <c r="I70" s="8">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="E8:E46" xr:uid="{57F1FF48-4396-4FE3-ABD9-234FB66F60F4}"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>

</xml_diff>

<commit_message>
Initial framework for plotting overall contribution of domestic manufacturing to toal demand
</commit_message>
<xml_diff>
--- a/fabrication_ports/ports_scenario.xlsx
+++ b/fabrication_ports/ports_scenario.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mshields\Documents\Projects\Supply Chain Roadmap\Analysis repos\Roadmap\fabrication_ports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{141152F6-F16F-4E22-B02C-323EF077D558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0FD4013-F9DA-4E58-B34A-BEBE89A4053B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Avg Demand Scenario" sheetId="9" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Avg Demand Scenario'!$E$8:$E$46</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Avg Demand Scenario'!$E$8:$E$47</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="24" r:id="rId2"/>
+    <pivotCache cacheId="27" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="176">
   <si>
     <t>Port</t>
   </si>
@@ -430,9 +430,6 @@
     <t>TBD - Coos Bay</t>
   </si>
   <si>
-    <t>TBD - WA</t>
-  </si>
-  <si>
     <t>WA</t>
   </si>
   <si>
@@ -454,9 +451,6 @@
     <t>Assembly port</t>
   </si>
   <si>
-    <t>Fabrication shipyard(new build)</t>
-  </si>
-  <si>
     <t>Semisubmersible 5</t>
   </si>
   <si>
@@ -466,12 +460,6 @@
     <t>TX</t>
   </si>
   <si>
-    <t>Fabrication shipyard (expand exising facility)</t>
-  </si>
-  <si>
-    <t>TBD - LA</t>
-  </si>
-  <si>
     <t>Semisubmersible 6</t>
   </si>
   <si>
@@ -556,16 +544,28 @@
     <t>Central Coast, CA</t>
   </si>
   <si>
-    <t>WA shipyard, WA</t>
-  </si>
-  <si>
-    <t>TX shipyard, TX</t>
-  </si>
-  <si>
     <t>TX port, TX</t>
   </si>
   <si>
-    <t>LA port, LA</t>
+    <t>Fabrication shipyard(new build). Suggest Columbia river gorge (near Vancouver, WA)</t>
+  </si>
+  <si>
+    <t>Fabrication shipyard (expand exising facility).  Suggest Kiewits facility in ….</t>
+  </si>
+  <si>
+    <t>Kiewit shipyard, TX</t>
+  </si>
+  <si>
+    <t>Vigor shipyard, WA</t>
+  </si>
+  <si>
+    <t>Vancouver, WA</t>
+  </si>
+  <si>
+    <t>Ingleside, TX</t>
+  </si>
+  <si>
+    <t>Semisubmersible 8</t>
   </si>
 </sst>
 </file>
@@ -767,17 +767,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Avg Demand Scenario'!$G$8</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Announcement date</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -788,9 +777,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Avg Demand Scenario'!$B$9:$B$35</c:f>
+              <c:f>'Avg Demand Scenario'!$B$9:$B$47</c:f>
               <c:strCache>
-                <c:ptCount val="27"/>
+                <c:ptCount val="39"/>
                 <c:pt idx="0">
                   <c:v>SGRE</c:v>
                 </c:pt>
@@ -871,16 +860,52 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>Steel plate 1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>Casting 1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>Flange 1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>Semisubmersible 1</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>Semisubmersible 2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>Semisubmersible 3</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>Semisubmersible 4</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>Semisubmersible 5</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>Semisubmersible 6</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>Semisubmersible 7</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>Semisubmersible 8</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>Mooring chain 1</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>Mooring rope 1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Avg Demand Scenario'!$G$9:$G$35</c:f>
+              <c:f>'Avg Demand Scenario'!$G$9:$G$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="39"/>
                 <c:pt idx="0">
                   <c:v>2021</c:v>
                 </c:pt>
@@ -961,6 +986,42 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2031</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2030</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2024</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -974,17 +1035,6 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Avg Demand Scenario'!$L$8</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Duration</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent2"/>
@@ -997,9 +1047,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Avg Demand Scenario'!$B$9:$B$35</c:f>
+              <c:f>'Avg Demand Scenario'!$B$9:$B$47</c:f>
               <c:strCache>
-                <c:ptCount val="27"/>
+                <c:ptCount val="39"/>
                 <c:pt idx="0">
                   <c:v>SGRE</c:v>
                 </c:pt>
@@ -1080,16 +1130,52 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>Steel plate 1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>Casting 1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>Flange 1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>Semisubmersible 1</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>Semisubmersible 2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>Semisubmersible 3</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>Semisubmersible 4</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>Semisubmersible 5</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>Semisubmersible 6</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>Semisubmersible 7</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>Semisubmersible 8</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>Mooring chain 1</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>Mooring rope 1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Avg Demand Scenario'!$L$9:$L$35</c:f>
+              <c:f>'Avg Demand Scenario'!$L$9:$L$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="39"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -1170,13 +1256,49 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-9625-4F3D-B07A-A2B748EFCD4C}"/>
+              <c16:uniqueId val="{00000000-E044-4197-B403-C30B0909D127}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1502,7 +1624,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Avg Demand Scenario'!$I$51</c:f>
+              <c:f>'Avg Demand Scenario'!$I$52</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1523,7 +1645,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Avg Demand Scenario'!$H$52:$H$70</c:f>
+              <c:f>'Avg Demand Scenario'!$H$53:$H$71</c:f>
               <c:strCache>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
@@ -1585,7 +1707,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Avg Demand Scenario'!$I$52:$I$70</c:f>
+              <c:f>'Avg Demand Scenario'!$I$53:$I$71</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
@@ -1605,10 +1727,10 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>2</c:v>
@@ -1617,7 +1739,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>4</c:v>
@@ -1635,7 +1757,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>1</c:v>
@@ -2965,14 +3087,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>30254</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>58177</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>209736</xdr:colOff>
-      <xdr:row>80</xdr:row>
-      <xdr:rowOff>75266</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>244928</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>54429</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3001,13 +3123,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>898921</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>75008</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>2458640</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>151208</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3037,15 +3159,18 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Shields, Matt" refreshedDate="44771.362389467591" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="39" xr:uid="{8520C2B9-52CF-46B0-8F6A-64DE6645DC34}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Shields, Matt" refreshedDate="44771.490716435183" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="39" xr:uid="{8520C2B9-52CF-46B0-8F6A-64DE6645DC34}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A8:L46" sheet="Avg Demand Scenario"/>
+    <worksheetSource ref="A8:L47" sheet="Avg Demand Scenario"/>
   </cacheSource>
-  <cacheFields count="11">
+  <cacheFields count="12">
     <cacheField name="Component" numFmtId="0">
       <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="Factory" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Name" numFmtId="0">
       <sharedItems/>
     </cacheField>
     <cacheField name="Port" numFmtId="0">
@@ -3055,6 +3180,7 @@
       <sharedItems count="18">
         <s v="VA"/>
         <s v="NC"/>
+        <s v="MA"/>
         <s v="NJ"/>
         <s v="OR"/>
         <s v="RI"/>
@@ -3063,7 +3189,6 @@
         <s v="MD"/>
         <s v="ME"/>
         <s v="LA"/>
-        <s v="MA"/>
         <s v="SC"/>
         <s v="KY"/>
         <s v="GA"/>
@@ -3108,6 +3233,7 @@
   <r>
     <s v="Blade"/>
     <s v="SGRE"/>
+    <s v="Portsmouth Marine Terminal, VA"/>
     <s v="Portsmouth Marine Terminal"/>
     <x v="0"/>
     <s v="South Atlantic"/>
@@ -3121,6 +3247,7 @@
   <r>
     <m/>
     <s v="Blade 1"/>
+    <s v="Port of Wilmington, NC"/>
     <s v="General Cargo Terminal at Port of Wilmington"/>
     <x v="1"/>
     <s v="South Atlantic"/>
@@ -3134,9 +3261,10 @@
   <r>
     <m/>
     <s v="Blade 2"/>
-    <s v="Newport News Marine Terminal"/>
-    <x v="0"/>
-    <s v="South Atlantic"/>
+    <s v="Mystic River, MA"/>
+    <s v="Mystic River, Everett"/>
+    <x v="2"/>
+    <s v="North Atlantic"/>
     <n v="2023"/>
     <n v="3"/>
     <n v="3"/>
@@ -3147,8 +3275,9 @@
   <r>
     <m/>
     <s v="Blade 3"/>
+    <s v="New Jersey Wind Port, NJ"/>
     <s v="New Jersey Wind Port"/>
-    <x v="2"/>
+    <x v="3"/>
     <s v="Central Atlantic"/>
     <n v="2023"/>
     <n v="3"/>
@@ -3160,8 +3289,9 @@
   <r>
     <m/>
     <s v="Blade 4"/>
+    <s v="Coos Bay, OR"/>
     <s v="TBD - Coos Bay"/>
-    <x v="3"/>
+    <x v="4"/>
     <s v="West Coast"/>
     <n v="2024"/>
     <n v="4"/>
@@ -3173,8 +3303,9 @@
   <r>
     <s v="Nacelle"/>
     <s v="GE"/>
+    <s v="New Jersey Wind Port, NJ"/>
     <s v="New Jersey Wind Port"/>
-    <x v="2"/>
+    <x v="3"/>
     <s v="Central Atlantic"/>
     <n v="2021"/>
     <n v="3"/>
@@ -3186,8 +3317,9 @@
   <r>
     <m/>
     <s v="Vestas"/>
+    <s v="New Jersey Wind Port, NJ"/>
     <s v="New Jersey Wind Port"/>
-    <x v="2"/>
+    <x v="3"/>
     <s v="Central Atlantic"/>
     <n v="2021"/>
     <n v="3"/>
@@ -3199,8 +3331,9 @@
   <r>
     <m/>
     <s v="Nacelle 1"/>
+    <s v="South Quay, RI"/>
     <s v="South Quay"/>
-    <x v="4"/>
+    <x v="5"/>
     <s v="North Atlantic"/>
     <n v="2023"/>
     <n v="3"/>
@@ -3212,8 +3345,9 @@
   <r>
     <m/>
     <s v="Nacelle 2"/>
+    <s v="Port of Humboldt, CA"/>
     <s v="TBD - Humboldt"/>
-    <x v="5"/>
+    <x v="6"/>
     <s v="West Coast"/>
     <n v="2023"/>
     <n v="4"/>
@@ -3225,8 +3359,9 @@
   <r>
     <s v="Tower"/>
     <s v="Marmen Welcon"/>
+    <s v="Port of Albany, NY"/>
     <s v="Port of Albany"/>
-    <x v="6"/>
+    <x v="7"/>
     <s v="Central Atlantic"/>
     <n v="2021"/>
     <n v="3"/>
@@ -3238,8 +3373,9 @@
   <r>
     <m/>
     <s v="Tower 1"/>
+    <s v="Tradepoint Atlantic, MD"/>
     <s v="Tradepoint Atlantic"/>
-    <x v="7"/>
+    <x v="8"/>
     <s v="South Atlantic"/>
     <n v="2023"/>
     <n v="3"/>
@@ -3251,8 +3387,9 @@
   <r>
     <m/>
     <s v="Tower 2"/>
+    <s v="Searsport, ME"/>
     <s v="Searsport"/>
-    <x v="8"/>
+    <x v="9"/>
     <s v="North Atlantic"/>
     <n v="2023"/>
     <n v="3"/>
@@ -3264,8 +3401,9 @@
   <r>
     <m/>
     <s v="Tower 3"/>
+    <s v="Port of Humboldt, CA"/>
     <s v="TBD - Humboldt"/>
-    <x v="5"/>
+    <x v="6"/>
     <s v="West Coast"/>
     <n v="2023"/>
     <n v="4"/>
@@ -3277,8 +3415,9 @@
   <r>
     <s v="Monopile"/>
     <s v="EEW"/>
+    <s v="Port of Paulsboro, NJ"/>
     <s v="Port of Paulsboro"/>
-    <x v="2"/>
+    <x v="3"/>
     <s v="Central Atlantic"/>
     <n v="2020"/>
     <n v="3"/>
@@ -3290,8 +3429,9 @@
   <r>
     <m/>
     <s v="US Wind"/>
+    <s v="Tradepoint Atlantic, MD"/>
     <s v="Tradepoint Atlantic"/>
-    <x v="2"/>
+    <x v="8"/>
     <s v="South Atlantic"/>
     <n v="2021"/>
     <n v="3"/>
@@ -3303,8 +3443,9 @@
   <r>
     <s v="Jacket"/>
     <s v="Jacket 1"/>
+    <s v="Port of New Orleans, LA"/>
     <s v="Port of New Orleans"/>
-    <x v="9"/>
+    <x v="10"/>
     <s v="Gulf of Mexico"/>
     <n v="2023"/>
     <n v="3"/>
@@ -3316,6 +3457,7 @@
   <r>
     <s v="GBF"/>
     <s v="GBF 1"/>
+    <s v="Radio Island, NC"/>
     <s v="Radio Island, Morehead City"/>
     <x v="1"/>
     <s v="South Atlantic"/>
@@ -3329,8 +3471,9 @@
   <r>
     <s v="Transition piece"/>
     <s v="Smulders"/>
+    <s v="Port of Albany, NY"/>
     <s v="Port of Albany"/>
-    <x v="6"/>
+    <x v="7"/>
     <s v="Central Atlantic"/>
     <n v="2021"/>
     <n v="3"/>
@@ -3342,8 +3485,9 @@
   <r>
     <m/>
     <s v="Transition piece 1"/>
+    <s v="Port of Coeymans, NY"/>
     <s v="Port of Coeymans"/>
-    <x v="6"/>
+    <x v="7"/>
     <s v="Central Atlantic"/>
     <n v="2023"/>
     <n v="3"/>
@@ -3355,8 +3499,9 @@
   <r>
     <s v="Array cable"/>
     <s v="Hellenic"/>
+    <s v="Tradepoint Atlantic, MD"/>
     <s v="Tradepoint Atlantic"/>
-    <x v="7"/>
+    <x v="8"/>
     <s v="South Atlantic"/>
     <n v="2021"/>
     <n v="3"/>
@@ -3368,22 +3513,10 @@
   <r>
     <m/>
     <s v="Array cable 1"/>
+    <s v="Arthur Kill Terminal, NY"/>
     <s v="Arthur Kill Terminal"/>
-    <x v="6"/>
+    <x v="7"/>
     <s v="Central Atlantic"/>
-    <n v="2023"/>
-    <n v="3"/>
-    <n v="5"/>
-    <n v="0.25"/>
-    <n v="2029"/>
-    <n v="6"/>
-  </r>
-  <r>
-    <m/>
-    <s v="Array cable 2"/>
-    <s v="Mystic River, Everett"/>
-    <x v="10"/>
-    <s v="North Atlantic"/>
     <n v="2023"/>
     <n v="3"/>
     <n v="5"/>
@@ -3394,6 +3527,7 @@
   <r>
     <s v="Export cable"/>
     <s v="Nexans"/>
+    <s v="Goose Island, SC"/>
     <s v="Goose Island"/>
     <x v="11"/>
     <s v="South Atlantic"/>
@@ -3407,8 +3541,9 @@
   <r>
     <m/>
     <s v="Prysmian"/>
+    <s v="Brayton Point, MA"/>
     <s v="Brayton Point"/>
-    <x v="10"/>
+    <x v="2"/>
     <s v="North Atlantic"/>
     <n v="2021"/>
     <n v="3"/>
@@ -3420,8 +3555,9 @@
   <r>
     <m/>
     <s v="Export cable 1"/>
+    <s v="Quonset Business Park, RI"/>
     <s v="Quonset Business Park / Port of Davisville"/>
-    <x v="4"/>
+    <x v="5"/>
     <s v="North Atlantic"/>
     <n v="2023"/>
     <n v="3"/>
@@ -3433,6 +3569,7 @@
   <r>
     <m/>
     <s v="Export cable 2"/>
+    <s v="Port of Charlotte, SC"/>
     <s v="Columbus Terminal"/>
     <x v="11"/>
     <s v="South Atlantic"/>
@@ -3446,6 +3583,7 @@
   <r>
     <s v="Steel plates"/>
     <s v="Nucor"/>
+    <s v="Brandenburg, KY"/>
     <s v="Brandenburg "/>
     <x v="12"/>
     <s v="South Atlantic"/>
@@ -3459,6 +3597,7 @@
   <r>
     <m/>
     <s v="Steel plate 1"/>
+    <s v="Port of Brunswick, GA"/>
     <s v="Port of Brunswick"/>
     <x v="13"/>
     <s v="South Atlantic"/>
@@ -3472,6 +3611,7 @@
   <r>
     <s v="Casting"/>
     <s v="Casting 1"/>
+    <s v="Inland facility, PA"/>
     <m/>
     <x v="14"/>
     <s v="Other"/>
@@ -3485,6 +3625,7 @@
   <r>
     <s v="Flange"/>
     <s v="Flange 1"/>
+    <s v="Portsmouth, NH"/>
     <s v="Schiller Newington, Portsmouth"/>
     <x v="15"/>
     <s v="North Atlantic"/>
@@ -3498,8 +3639,9 @@
   <r>
     <s v="Semisubmersible"/>
     <s v="Semisubmersible 1"/>
+    <s v="Port of Humboldt, CA"/>
     <s v="TBD - Humboldt"/>
-    <x v="5"/>
+    <x v="6"/>
     <s v="West Coast"/>
     <n v="2024"/>
     <n v="4"/>
@@ -3511,8 +3653,9 @@
   <r>
     <m/>
     <s v="Semisubmersible 2"/>
+    <s v="Central Coast, CA"/>
     <s v="TBD - Central Coast"/>
-    <x v="5"/>
+    <x v="6"/>
     <s v="West Coast"/>
     <n v="2025"/>
     <n v="4"/>
@@ -3524,8 +3667,9 @@
   <r>
     <m/>
     <s v="Semisubmersible 3"/>
+    <s v="Coos Bay, OR"/>
     <s v="TBD - Coos Bay"/>
-    <x v="3"/>
+    <x v="4"/>
     <s v="West Coast"/>
     <n v="2026"/>
     <n v="4"/>
@@ -3537,8 +3681,9 @@
   <r>
     <m/>
     <s v="Semisubmersible 4"/>
+    <s v="Port of New Orleans, LA"/>
     <s v="Port of New Orleans"/>
-    <x v="9"/>
+    <x v="10"/>
     <s v="Gulf of Mexico"/>
     <n v="2031"/>
     <n v="2"/>
@@ -3550,6 +3695,7 @@
   <r>
     <m/>
     <s v="Semisubmersible 5"/>
+    <s v="Portsmouth Marine Terminal, VA"/>
     <s v="Portsmouth Marine Terminal"/>
     <x v="0"/>
     <s v="South Atlantic"/>
@@ -3563,7 +3709,22 @@
   <r>
     <m/>
     <s v="Semisubmersible 6"/>
-    <s v="TBD - WA"/>
+    <s v="Searsport, ME"/>
+    <s v="Searsport"/>
+    <x v="9"/>
+    <s v="North Atlantic"/>
+    <n v="2029"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="0.25"/>
+    <n v="2031"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <m/>
+    <s v="Semisubmersible 7"/>
+    <s v="Vigor shipyard, WA"/>
+    <s v="Vancouver, WA"/>
     <x v="16"/>
     <s v="West Coast"/>
     <n v="2024"/>
@@ -3575,8 +3736,9 @@
   </r>
   <r>
     <m/>
-    <s v="Semisubmersible 7"/>
-    <s v="TBD - TX"/>
+    <s v="Semisubmersible 8"/>
+    <s v="Kiewit shipyard, TX"/>
+    <s v="Ingleside, TX"/>
     <x v="17"/>
     <s v="Gulf of Mexico"/>
     <n v="2028"/>
@@ -3589,6 +3751,7 @@
   <r>
     <s v="Stationkeeping"/>
     <s v="Mooring chain 1"/>
+    <s v="TX port, TX"/>
     <s v="TBD - TX"/>
     <x v="17"/>
     <s v="Gulf of Mexico"/>
@@ -3602,8 +3765,9 @@
   <r>
     <m/>
     <s v="Mooring rope 1"/>
-    <s v="TBD - LA"/>
-    <x v="9"/>
+    <s v="Port of New Orleans, LA"/>
+    <s v="Port of New Orleans"/>
+    <x v="10"/>
     <s v="Gulf of Mexico"/>
     <n v="2024"/>
     <n v="3"/>
@@ -3616,28 +3780,29 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5CA5F775-FB12-4A7B-98B7-3842EC7091C4}" name="PivotTable1" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
-  <location ref="H51:I70" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="11">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5CA5F775-FB12-4A7B-98B7-3842EC7091C4}" name="PivotTable1" cacheId="27" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+  <location ref="H52:I71" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="12">
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
     <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
       <items count="19">
-        <item x="5"/>
+        <item x="6"/>
         <item x="13"/>
         <item x="12"/>
+        <item x="10"/>
+        <item x="2"/>
+        <item x="8"/>
         <item x="9"/>
-        <item x="10"/>
-        <item x="7"/>
-        <item x="8"/>
         <item x="1"/>
         <item x="15"/>
-        <item x="2"/>
-        <item x="6"/>
         <item x="3"/>
+        <item x="7"/>
+        <item x="4"/>
         <item x="14"/>
-        <item x="4"/>
+        <item x="5"/>
         <item x="11"/>
         <item x="0"/>
         <item x="16"/>
@@ -3654,7 +3819,7 @@
     <pivotField showAll="0"/>
   </pivotFields>
   <rowFields count="1">
-    <field x="3"/>
+    <field x="4"/>
   </rowFields>
   <rowItems count="19">
     <i>
@@ -4029,10 +4194,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F1FF48-4396-4FE3-ABD9-234FB66F60F4}">
-  <dimension ref="A1:M70"/>
+  <dimension ref="A1:M71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="J86" sqref="J86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4043,8 +4208,8 @@
     <col min="5" max="5" width="12.42578125" customWidth="1"/>
     <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.28515625" bestFit="1" customWidth="1"/>
@@ -4117,7 +4282,7 @@
         <v>33</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>0</v>
@@ -4158,7 +4323,7 @@
         <v>42</v>
       </c>
       <c r="C9" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
@@ -4197,7 +4362,7 @@
         <v>43</v>
       </c>
       <c r="C10" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>9</v>
@@ -4227,7 +4392,7 @@
         <v>2028</v>
       </c>
       <c r="L10">
-        <f t="shared" ref="L10:L46" si="1">K10-G10</f>
+        <f t="shared" ref="L10:L47" si="1">K10-G10</f>
         <v>5</v>
       </c>
       <c r="M10" t="s">
@@ -4239,7 +4404,7 @@
         <v>45</v>
       </c>
       <c r="C11" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>20</v>
@@ -4265,7 +4430,7 @@
         <v>0.25</v>
       </c>
       <c r="K11">
-        <f t="shared" ref="K11:K46" si="2">ROUNDDOWN(G11+H11+I11*(1-J11),0)</f>
+        <f t="shared" ref="K11:K47" si="2">ROUNDDOWN(G11+H11+I11*(1-J11),0)</f>
         <v>2028</v>
       </c>
       <c r="L11">
@@ -4281,7 +4446,7 @@
         <v>46</v>
       </c>
       <c r="C12" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>47</v>
@@ -4323,7 +4488,7 @@
         <v>121</v>
       </c>
       <c r="C13" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>129</v>
@@ -4364,7 +4529,7 @@
         <v>50</v>
       </c>
       <c r="C14" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D14" t="s">
         <v>47</v>
@@ -4406,7 +4571,7 @@
         <v>51</v>
       </c>
       <c r="C15" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D15" t="s">
         <v>47</v>
@@ -4448,7 +4613,7 @@
         <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>29</v>
@@ -4487,7 +4652,7 @@
         <v>123</v>
       </c>
       <c r="C17" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>127</v>
@@ -4527,7 +4692,7 @@
         <v>54</v>
       </c>
       <c r="C18" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>25</v>
@@ -4568,7 +4733,7 @@
         <v>56</v>
       </c>
       <c r="C19" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>57</v>
@@ -4610,7 +4775,7 @@
         <v>59</v>
       </c>
       <c r="C20" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>18</v>
@@ -4652,7 +4817,7 @@
         <v>124</v>
       </c>
       <c r="C21" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>127</v>
@@ -4693,7 +4858,7 @@
         <v>62</v>
       </c>
       <c r="C22" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>27</v>
@@ -4734,7 +4899,7 @@
         <v>63</v>
       </c>
       <c r="C23" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>57</v>
@@ -4779,7 +4944,7 @@
         <v>66</v>
       </c>
       <c r="C24" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>21</v>
@@ -4824,7 +4989,7 @@
         <v>106</v>
       </c>
       <c r="C25" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>86</v>
@@ -4867,7 +5032,7 @@
         <v>70</v>
       </c>
       <c r="C26" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>25</v>
@@ -4908,7 +5073,7 @@
         <v>108</v>
       </c>
       <c r="C27" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>71</v>
@@ -4953,7 +5118,7 @@
         <v>74</v>
       </c>
       <c r="C28" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>57</v>
@@ -4992,7 +5157,7 @@
         <v>75</v>
       </c>
       <c r="C29" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>28</v>
@@ -5037,7 +5202,7 @@
         <v>78</v>
       </c>
       <c r="C30" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>79</v>
@@ -5077,7 +5242,7 @@
         <v>82</v>
       </c>
       <c r="C31" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>13</v>
@@ -5116,7 +5281,7 @@
         <v>83</v>
       </c>
       <c r="C32" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>16</v>
@@ -5158,7 +5323,7 @@
         <v>85</v>
       </c>
       <c r="C33" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D33" t="s">
         <v>11</v>
@@ -5200,7 +5365,7 @@
         <v>88</v>
       </c>
       <c r="C34" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>89</v>
@@ -5239,7 +5404,7 @@
         <v>91</v>
       </c>
       <c r="C35" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D35" t="s">
         <v>3</v>
@@ -5281,7 +5446,7 @@
         <v>110</v>
       </c>
       <c r="C36" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E36" t="s">
         <v>111</v>
@@ -5315,19 +5480,19 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>131</v>
+      </c>
+      <c r="B37" t="s">
         <v>132</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
+        <v>166</v>
+      </c>
+      <c r="D37" t="s">
+        <v>134</v>
+      </c>
+      <c r="E37" t="s">
         <v>133</v>
-      </c>
-      <c r="C37" t="s">
-        <v>170</v>
-      </c>
-      <c r="D37" t="s">
-        <v>135</v>
-      </c>
-      <c r="E37" t="s">
-        <v>134</v>
       </c>
       <c r="F37" t="s">
         <v>15</v>
@@ -5361,7 +5526,7 @@
         <v>115</v>
       </c>
       <c r="C38" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D38" t="s">
         <v>127</v>
@@ -5393,7 +5558,7 @@
         <v>4</v>
       </c>
       <c r="M38" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
@@ -5401,7 +5566,7 @@
         <v>116</v>
       </c>
       <c r="C39" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D39" t="s">
         <v>128</v>
@@ -5433,7 +5598,7 @@
         <v>4</v>
       </c>
       <c r="M39" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
@@ -5441,7 +5606,7 @@
         <v>117</v>
       </c>
       <c r="C40" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D40" t="s">
         <v>129</v>
@@ -5473,15 +5638,15 @@
         <v>4</v>
       </c>
       <c r="M40" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C41" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D41" t="s">
         <v>21</v>
@@ -5513,15 +5678,15 @@
         <v>2</v>
       </c>
       <c r="M41" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C42" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D42" t="s">
         <v>7</v>
@@ -5553,70 +5718,70 @@
         <v>2</v>
       </c>
       <c r="M42" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C43" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="D43" t="s">
-        <v>130</v>
+        <v>18</v>
       </c>
       <c r="E43" t="s">
-        <v>131</v>
+        <v>19</v>
       </c>
       <c r="F43" t="s">
-        <v>126</v>
+        <v>15</v>
       </c>
       <c r="G43">
-        <v>2024</v>
+        <v>2029</v>
       </c>
       <c r="H43">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I43">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J43">
         <v>0.25</v>
       </c>
       <c r="K43">
-        <f t="shared" ref="K43:K44" si="14">ROUNDDOWN(G43+H43+I43*(1-J43),0)</f>
-        <v>2028</v>
+        <f t="shared" ref="K43" si="14">ROUNDDOWN(G43+H43+I43*(1-J43),0)</f>
+        <v>2031</v>
       </c>
       <c r="L43">
-        <f t="shared" ref="L43:L44" si="15">K43-G43</f>
-        <v>4</v>
+        <f t="shared" ref="L43" si="15">K43-G43</f>
+        <v>2</v>
       </c>
       <c r="M43" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C44" t="s">
+        <v>172</v>
+      </c>
+      <c r="D44" t="s">
         <v>173</v>
       </c>
-      <c r="D44" t="s">
-        <v>140</v>
-      </c>
       <c r="E44" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="F44" t="s">
-        <v>67</v>
+        <v>126</v>
       </c>
       <c r="G44">
-        <v>2028</v>
+        <v>2024</v>
       </c>
       <c r="H44">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I44">
         <v>2</v>
@@ -5625,41 +5790,38 @@
         <v>0.25</v>
       </c>
       <c r="K44">
-        <f t="shared" si="14"/>
-        <v>2031</v>
+        <f t="shared" ref="K44:K45" si="16">ROUNDDOWN(G44+H44+I44*(1-J44),0)</f>
+        <v>2028</v>
       </c>
       <c r="L44">
-        <f t="shared" si="15"/>
-        <v>3</v>
+        <f t="shared" ref="L44:L45" si="17">K44-G44</f>
+        <v>4</v>
       </c>
       <c r="M44" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>118</v>
-      </c>
       <c r="B45" t="s">
-        <v>119</v>
+        <v>175</v>
       </c>
       <c r="C45" t="s">
+        <v>171</v>
+      </c>
+      <c r="D45" t="s">
         <v>174</v>
       </c>
-      <c r="D45" t="s">
-        <v>140</v>
-      </c>
       <c r="E45" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F45" t="s">
         <v>67</v>
       </c>
       <c r="G45">
-        <v>2024</v>
+        <v>2028</v>
       </c>
       <c r="H45">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I45">
         <v>2</v>
@@ -5668,29 +5830,32 @@
         <v>0.25</v>
       </c>
       <c r="K45">
-        <f t="shared" si="2"/>
-        <v>2028</v>
+        <f t="shared" si="16"/>
+        <v>2031</v>
       </c>
       <c r="L45">
-        <f t="shared" si="1"/>
-        <v>4</v>
+        <f t="shared" si="17"/>
+        <v>3</v>
       </c>
       <c r="M45" t="s">
-        <v>146</v>
+        <v>170</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>118</v>
+      </c>
       <c r="B46" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C46" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="D46" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="E46" t="s">
-        <v>22</v>
+        <v>139</v>
       </c>
       <c r="F46" t="s">
         <v>67</v>
@@ -5716,41 +5881,73 @@
         <v>4</v>
       </c>
       <c r="M46" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>120</v>
+      </c>
+      <c r="C47" t="s">
+        <v>155</v>
+      </c>
+      <c r="D47" t="s">
+        <v>21</v>
+      </c>
+      <c r="E47" t="s">
+        <v>22</v>
+      </c>
+      <c r="F47" t="s">
+        <v>67</v>
+      </c>
+      <c r="G47">
+        <v>2024</v>
+      </c>
+      <c r="H47">
+        <v>3</v>
+      </c>
+      <c r="I47">
+        <v>2</v>
+      </c>
+      <c r="J47">
+        <v>0.25</v>
+      </c>
+      <c r="K47">
+        <f t="shared" si="2"/>
+        <v>2028</v>
+      </c>
+      <c r="L47">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="M47" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H51" s="6" t="s">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H52" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="I51" t="s">
+      <c r="I52" t="s">
         <v>104</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H52" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="I52" s="8">
-        <v>4</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H53" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="I53" s="8">
         <v>4</v>
-      </c>
-      <c r="I53" s="8">
-        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H54" s="7" t="s">
-        <v>90</v>
+        <v>4</v>
       </c>
       <c r="I54" s="8">
         <v>1</v>
@@ -5758,23 +5955,23 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H55" s="7" t="s">
-        <v>22</v>
+        <v>90</v>
       </c>
       <c r="I55" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H56" s="7" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="I56" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H57" s="7" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="I57" s="8">
         <v>2</v>
@@ -5782,15 +5979,15 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H58" s="7" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="I58" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H59" s="7" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="I59" s="8">
         <v>2</v>
@@ -5798,23 +5995,23 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H60" s="7" t="s">
-        <v>134</v>
+        <v>10</v>
       </c>
       <c r="I60" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H61" s="7" t="s">
-        <v>26</v>
+        <v>133</v>
       </c>
       <c r="I61" s="8">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H62" s="7" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="I62" s="8">
         <v>4</v>
@@ -5822,31 +6019,31 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H63" s="7" t="s">
-        <v>125</v>
+        <v>23</v>
       </c>
       <c r="I63" s="8">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H64" s="7" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="I64" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="65" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H65" s="7" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="I65" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H66" s="7" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="I66" s="8">
         <v>2</v>
@@ -5854,38 +6051,46 @@
     </row>
     <row r="67" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H67" s="7" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I67" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H68" s="7" t="s">
-        <v>131</v>
+        <v>8</v>
       </c>
       <c r="I68" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="69" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H69" s="7" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="I69" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H70" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="I70" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H71" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="I70" s="8">
+      <c r="I71" s="8">
         <v>39</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="E8:E46" xr:uid="{57F1FF48-4396-4FE3-ABD9-234FB66F60F4}"/>
+  <autoFilter ref="E8:E47" xr:uid="{57F1FF48-4396-4FE3-ABD9-234FB66F60F4}"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>

</xml_diff>

<commit_message>
Revised overall gantt chart ordering, naming, coloring
</commit_message>
<xml_diff>
--- a/fabrication_ports/ports_scenario.xlsx
+++ b/fabrication_ports/ports_scenario.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mshields\Documents\Projects\Supply Chain Roadmap\Analysis repos\Roadmap\fabrication_ports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0FD4013-F9DA-4E58-B34A-BEBE89A4053B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C1AEAC-062D-4A75-8FCE-1FBC26693321}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Avg Demand Scenario" sheetId="9" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Avg Demand Scenario'!$E$8:$E$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Avg Demand Scenario'!$E$8:$E$45</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="27" r:id="rId2"/>
+    <pivotCache cacheId="22" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="168">
   <si>
     <t>Port</t>
   </si>
@@ -463,9 +463,6 @@
     <t>Semisubmersible 6</t>
   </si>
   <si>
-    <t>Semisubmersible 7</t>
-  </si>
-  <si>
     <t>Service WC and EC</t>
   </si>
   <si>
@@ -545,27 +542,6 @@
   </si>
   <si>
     <t>TX port, TX</t>
-  </si>
-  <si>
-    <t>Fabrication shipyard(new build). Suggest Columbia river gorge (near Vancouver, WA)</t>
-  </si>
-  <si>
-    <t>Fabrication shipyard (expand exising facility).  Suggest Kiewits facility in ….</t>
-  </si>
-  <si>
-    <t>Kiewit shipyard, TX</t>
-  </si>
-  <si>
-    <t>Vigor shipyard, WA</t>
-  </si>
-  <si>
-    <t>Vancouver, WA</t>
-  </si>
-  <si>
-    <t>Ingleside, TX</t>
-  </si>
-  <si>
-    <t>Semisubmersible 8</t>
   </si>
 </sst>
 </file>
@@ -777,9 +753,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Avg Demand Scenario'!$B$9:$B$47</c:f>
+              <c:f>'Avg Demand Scenario'!$B$9:$B$45</c:f>
               <c:strCache>
-                <c:ptCount val="39"/>
+                <c:ptCount val="37"/>
                 <c:pt idx="0">
                   <c:v>SGRE</c:v>
                 </c:pt>
@@ -886,15 +862,9 @@
                   <c:v>Semisubmersible 6</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>Semisubmersible 7</c:v>
+                  <c:v>Mooring chain 1</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>Semisubmersible 8</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>Mooring chain 1</c:v>
-                </c:pt>
-                <c:pt idx="38">
                   <c:v>Mooring rope 1</c:v>
                 </c:pt>
               </c:strCache>
@@ -902,10 +872,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Avg Demand Scenario'!$G$9:$G$47</c:f>
+              <c:f>'Avg Demand Scenario'!$G$9:$G$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="39"/>
+                <c:ptCount val="37"/>
                 <c:pt idx="0">
                   <c:v>2021</c:v>
                 </c:pt>
@@ -1015,12 +985,6 @@
                   <c:v>2024</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2028</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>2024</c:v>
-                </c:pt>
-                <c:pt idx="38">
                   <c:v>2024</c:v>
                 </c:pt>
               </c:numCache>
@@ -1047,9 +1011,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Avg Demand Scenario'!$B$9:$B$47</c:f>
+              <c:f>'Avg Demand Scenario'!$B$9:$B$45</c:f>
               <c:strCache>
-                <c:ptCount val="39"/>
+                <c:ptCount val="37"/>
                 <c:pt idx="0">
                   <c:v>SGRE</c:v>
                 </c:pt>
@@ -1156,15 +1120,9 @@
                   <c:v>Semisubmersible 6</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>Semisubmersible 7</c:v>
+                  <c:v>Mooring chain 1</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>Semisubmersible 8</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>Mooring chain 1</c:v>
-                </c:pt>
-                <c:pt idx="38">
                   <c:v>Mooring rope 1</c:v>
                 </c:pt>
               </c:strCache>
@@ -1172,10 +1130,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Avg Demand Scenario'!$L$9:$L$47</c:f>
+              <c:f>'Avg Demand Scenario'!$L$9:$L$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="39"/>
+                <c:ptCount val="37"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -1285,12 +1243,6 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="38">
                   <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
@@ -1624,7 +1576,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Avg Demand Scenario'!$I$52</c:f>
+              <c:f>'Avg Demand Scenario'!$I$50</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1645,7 +1597,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Avg Demand Scenario'!$H$53:$H$71</c:f>
+              <c:f>'Avg Demand Scenario'!$H$51:$H$69</c:f>
               <c:strCache>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
@@ -1707,7 +1659,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Avg Demand Scenario'!$I$53:$I$71</c:f>
+              <c:f>'Avg Demand Scenario'!$I$51:$I$69</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
@@ -3087,13 +3039,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>30254</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>58177</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>244928</xdr:colOff>
-      <xdr:row>96</xdr:row>
+      <xdr:row>94</xdr:row>
       <xdr:rowOff>54429</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3123,13 +3075,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>898921</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>75008</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>2458640</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>151208</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3161,7 +3113,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Shields, Matt" refreshedDate="44771.490716435183" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="39" xr:uid="{8520C2B9-52CF-46B0-8F6A-64DE6645DC34}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A8:L47" sheet="Avg Demand Scenario"/>
+    <worksheetSource ref="A8:L45" sheet="Avg Demand Scenario"/>
   </cacheSource>
   <cacheFields count="12">
     <cacheField name="Component" numFmtId="0">
@@ -3780,8 +3732,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5CA5F775-FB12-4A7B-98B7-3842EC7091C4}" name="PivotTable1" cacheId="27" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
-  <location ref="H52:I71" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5CA5F775-FB12-4A7B-98B7-3842EC7091C4}" name="PivotTable1" cacheId="22" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+  <location ref="H50:I69" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
@@ -4194,34 +4146,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F1FF48-4396-4FE3-ABD9-234FB66F60F4}">
-  <dimension ref="A1:M71"/>
+  <dimension ref="A1:M69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="J86" sqref="J86"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44:XFD45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="25.140625" customWidth="1"/>
-    <col min="4" max="4" width="42.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="82.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="25.1796875" customWidth="1"/>
+    <col min="4" max="4" width="42.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.453125" customWidth="1"/>
+    <col min="6" max="6" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="82.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>93</v>
       </c>
@@ -4235,7 +4187,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>34</v>
       </c>
@@ -4246,7 +4198,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>99</v>
       </c>
@@ -4257,7 +4209,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
@@ -4274,7 +4226,7 @@
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>32</v>
       </c>
@@ -4282,7 +4234,7 @@
         <v>33</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>0</v>
@@ -4315,7 +4267,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -4323,7 +4275,7 @@
         <v>42</v>
       </c>
       <c r="C9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
@@ -4357,12 +4309,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>43</v>
       </c>
       <c r="C10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>9</v>
@@ -4392,19 +4344,19 @@
         <v>2028</v>
       </c>
       <c r="L10">
-        <f t="shared" ref="L10:L47" si="1">K10-G10</f>
+        <f t="shared" ref="L10:L45" si="1">K10-G10</f>
         <v>5</v>
       </c>
       <c r="M10" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>45</v>
       </c>
       <c r="C11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>20</v>
@@ -4430,7 +4382,7 @@
         <v>0.25</v>
       </c>
       <c r="K11">
-        <f t="shared" ref="K11:K47" si="2">ROUNDDOWN(G11+H11+I11*(1-J11),0)</f>
+        <f t="shared" ref="K11:K45" si="2">ROUNDDOWN(G11+H11+I11*(1-J11),0)</f>
         <v>2028</v>
       </c>
       <c r="L11">
@@ -4441,12 +4393,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>46</v>
       </c>
       <c r="C12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>47</v>
@@ -4483,12 +4435,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>121</v>
       </c>
       <c r="C13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>129</v>
@@ -4521,7 +4473,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>49</v>
       </c>
@@ -4529,7 +4481,7 @@
         <v>50</v>
       </c>
       <c r="C14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D14" t="s">
         <v>47</v>
@@ -4566,12 +4518,12 @@
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>51</v>
       </c>
       <c r="C15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D15" t="s">
         <v>47</v>
@@ -4608,12 +4560,12 @@
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>29</v>
@@ -4647,12 +4599,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>123</v>
       </c>
       <c r="C17" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>127</v>
@@ -4684,7 +4636,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>53</v>
       </c>
@@ -4692,7 +4644,7 @@
         <v>54</v>
       </c>
       <c r="C18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>25</v>
@@ -4728,12 +4680,12 @@
         <v>97</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>56</v>
       </c>
       <c r="C19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>57</v>
@@ -4770,12 +4722,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>59</v>
       </c>
       <c r="C20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>18</v>
@@ -4812,12 +4764,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>124</v>
       </c>
       <c r="C21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>127</v>
@@ -4850,7 +4802,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>61</v>
       </c>
@@ -4858,7 +4810,7 @@
         <v>62</v>
       </c>
       <c r="C22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>27</v>
@@ -4894,12 +4846,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>63</v>
       </c>
       <c r="C23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>57</v>
@@ -4936,7 +4888,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>65</v>
       </c>
@@ -4944,7 +4896,7 @@
         <v>66</v>
       </c>
       <c r="C24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>21</v>
@@ -4981,7 +4933,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>105</v>
       </c>
@@ -4989,7 +4941,7 @@
         <v>106</v>
       </c>
       <c r="C25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>86</v>
@@ -5024,7 +4976,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>69</v>
       </c>
@@ -5032,7 +4984,7 @@
         <v>70</v>
       </c>
       <c r="C26" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>25</v>
@@ -5047,7 +4999,7 @@
         <v>2021</v>
       </c>
       <c r="H26">
-        <f>$D$5</f>
+        <f t="shared" ref="H26:H35" si="10">$D$5</f>
         <v>3</v>
       </c>
       <c r="I26">
@@ -5068,12 +5020,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>108</v>
       </c>
       <c r="C27" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>71</v>
@@ -5088,14 +5040,14 @@
         <v>2023</v>
       </c>
       <c r="H27">
-        <f>$D$5</f>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
       <c r="I27">
         <v>2.5</v>
       </c>
       <c r="J27">
-        <f t="shared" ref="J27:J29" si="10">$D$3</f>
+        <f t="shared" ref="J27:J29" si="11">$D$3</f>
         <v>0.25</v>
       </c>
       <c r="K27">
@@ -5110,7 +5062,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>73</v>
       </c>
@@ -5118,7 +5070,7 @@
         <v>74</v>
       </c>
       <c r="C28" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>57</v>
@@ -5133,14 +5085,14 @@
         <v>2021</v>
       </c>
       <c r="H28">
-        <f>$D$5</f>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
       <c r="I28">
         <v>5</v>
       </c>
       <c r="J28">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.25</v>
       </c>
       <c r="K28">
@@ -5152,12 +5104,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>75</v>
       </c>
       <c r="C29" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>28</v>
@@ -5172,14 +5124,14 @@
         <v>2023</v>
       </c>
       <c r="H29">
-        <f>$D$5</f>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
       <c r="I29">
         <v>5</v>
       </c>
       <c r="J29">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.25</v>
       </c>
       <c r="K29">
@@ -5194,7 +5146,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>77</v>
       </c>
@@ -5202,7 +5154,7 @@
         <v>78</v>
       </c>
       <c r="C30" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>79</v>
@@ -5217,7 +5169,7 @@
         <v>2018</v>
       </c>
       <c r="H30">
-        <f>$D$5</f>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
       <c r="I30" t="s">
@@ -5237,12 +5189,12 @@
         <v>81</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>82</v>
       </c>
       <c r="C31" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>13</v>
@@ -5257,14 +5209,14 @@
         <v>2021</v>
       </c>
       <c r="H31">
-        <f>$D$5</f>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
       <c r="I31">
         <v>5</v>
       </c>
       <c r="J31">
-        <f t="shared" ref="J31:J35" si="11">$D$3</f>
+        <f t="shared" ref="J31:J35" si="12">$D$3</f>
         <v>0.25</v>
       </c>
       <c r="K31">
@@ -5276,12 +5228,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>83</v>
       </c>
       <c r="C32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>16</v>
@@ -5296,14 +5248,14 @@
         <v>2023</v>
       </c>
       <c r="H32">
-        <f>$D$5</f>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
       <c r="I32">
         <v>5</v>
       </c>
       <c r="J32">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.25</v>
       </c>
       <c r="K32">
@@ -5318,12 +5270,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
         <v>85</v>
       </c>
       <c r="C33" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D33" t="s">
         <v>11</v>
@@ -5338,14 +5290,14 @@
         <v>2023</v>
       </c>
       <c r="H33">
-        <f>$D$5</f>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
       <c r="I33">
         <v>5</v>
       </c>
       <c r="J33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.25</v>
       </c>
       <c r="K33">
@@ -5357,7 +5309,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>87</v>
       </c>
@@ -5365,7 +5317,7 @@
         <v>88</v>
       </c>
       <c r="C34" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>89</v>
@@ -5380,14 +5332,14 @@
         <v>2021</v>
       </c>
       <c r="H34">
-        <f>$D$5</f>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
       <c r="I34">
         <v>2</v>
       </c>
       <c r="J34">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.25</v>
       </c>
       <c r="K34">
@@ -5399,12 +5351,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
         <v>91</v>
       </c>
       <c r="C35" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D35" t="s">
         <v>3</v>
@@ -5419,14 +5371,14 @@
         <v>2023</v>
       </c>
       <c r="H35">
-        <f>$D$5</f>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
       <c r="I35">
         <v>5</v>
       </c>
       <c r="J35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.25</v>
       </c>
       <c r="K35">
@@ -5438,7 +5390,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>109</v>
       </c>
@@ -5446,7 +5398,7 @@
         <v>110</v>
       </c>
       <c r="C36" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E36" t="s">
         <v>111</v>
@@ -5478,7 +5430,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>131</v>
       </c>
@@ -5486,7 +5438,7 @@
         <v>132</v>
       </c>
       <c r="C37" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D37" t="s">
         <v>134</v>
@@ -5518,7 +5470,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>114</v>
       </c>
@@ -5526,7 +5478,7 @@
         <v>115</v>
       </c>
       <c r="C38" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D38" t="s">
         <v>127</v>
@@ -5561,12 +5513,12 @@
         <v>136</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B39" t="s">
         <v>116</v>
       </c>
       <c r="C39" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D39" t="s">
         <v>128</v>
@@ -5601,12 +5553,12 @@
         <v>136</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B40" t="s">
         <v>117</v>
       </c>
       <c r="C40" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D40" t="s">
         <v>129</v>
@@ -5641,12 +5593,12 @@
         <v>136</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
         <v>135</v>
       </c>
       <c r="C41" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D41" t="s">
         <v>21</v>
@@ -5670,23 +5622,23 @@
         <v>0.25</v>
       </c>
       <c r="K41">
-        <f t="shared" ref="K41:K42" si="12">ROUNDDOWN(G41+H41+I41*(1-J41),0)</f>
+        <f t="shared" ref="K41:K42" si="13">ROUNDDOWN(G41+H41+I41*(1-J41),0)</f>
         <v>2033</v>
       </c>
       <c r="L41">
-        <f t="shared" ref="L41:L42" si="13">K41-G41</f>
+        <f t="shared" ref="L41:L42" si="14">K41-G41</f>
         <v>2</v>
       </c>
       <c r="M41" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
         <v>137</v>
       </c>
       <c r="C42" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D42" t="s">
         <v>7</v>
@@ -5710,23 +5662,23 @@
         <v>0.25</v>
       </c>
       <c r="K42">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2032</v>
       </c>
       <c r="L42">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="M42" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
         <v>140</v>
       </c>
       <c r="C43" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D43" t="s">
         <v>18</v>
@@ -5750,32 +5702,35 @@
         <v>0.25</v>
       </c>
       <c r="K43">
-        <f t="shared" ref="K43" si="14">ROUNDDOWN(G43+H43+I43*(1-J43),0)</f>
+        <f t="shared" ref="K43" si="15">ROUNDDOWN(G43+H43+I43*(1-J43),0)</f>
         <v>2031</v>
       </c>
       <c r="L43">
-        <f t="shared" ref="L43" si="15">K43-G43</f>
+        <f t="shared" ref="L43" si="16">K43-G43</f>
         <v>2</v>
       </c>
       <c r="M43" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>118</v>
+      </c>
       <c r="B44" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="C44" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="D44" t="s">
-        <v>173</v>
+        <v>138</v>
       </c>
       <c r="E44" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="F44" t="s">
-        <v>126</v>
+        <v>67</v>
       </c>
       <c r="G44">
         <v>2024</v>
@@ -5790,38 +5745,38 @@
         <v>0.25</v>
       </c>
       <c r="K44">
-        <f t="shared" ref="K44:K45" si="16">ROUNDDOWN(G44+H44+I44*(1-J44),0)</f>
+        <f t="shared" si="2"/>
         <v>2028</v>
       </c>
       <c r="L44">
-        <f t="shared" ref="L44:L45" si="17">K44-G44</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="M44" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B45" t="s">
-        <v>175</v>
+        <v>120</v>
       </c>
       <c r="C45" t="s">
-        <v>171</v>
+        <v>154</v>
       </c>
       <c r="D45" t="s">
-        <v>174</v>
+        <v>21</v>
       </c>
       <c r="E45" t="s">
-        <v>139</v>
+        <v>22</v>
       </c>
       <c r="F45" t="s">
         <v>67</v>
       </c>
       <c r="G45">
-        <v>2028</v>
+        <v>2024</v>
       </c>
       <c r="H45">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I45">
         <v>2</v>
@@ -5830,267 +5785,184 @@
         <v>0.25</v>
       </c>
       <c r="K45">
-        <f t="shared" si="16"/>
-        <v>2031</v>
-      </c>
-      <c r="L45">
-        <f t="shared" si="17"/>
-        <v>3</v>
-      </c>
-      <c r="M45" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>118</v>
-      </c>
-      <c r="B46" t="s">
-        <v>119</v>
-      </c>
-      <c r="C46" t="s">
-        <v>168</v>
-      </c>
-      <c r="D46" t="s">
-        <v>138</v>
-      </c>
-      <c r="E46" t="s">
-        <v>139</v>
-      </c>
-      <c r="F46" t="s">
-        <v>67</v>
-      </c>
-      <c r="G46">
-        <v>2024</v>
-      </c>
-      <c r="H46">
-        <v>3</v>
-      </c>
-      <c r="I46">
-        <v>2</v>
-      </c>
-      <c r="J46">
-        <v>0.25</v>
-      </c>
-      <c r="K46">
         <f t="shared" si="2"/>
         <v>2028</v>
       </c>
-      <c r="L46">
+      <c r="L45">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="M46" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>120</v>
-      </c>
-      <c r="C47" t="s">
-        <v>155</v>
-      </c>
-      <c r="D47" t="s">
-        <v>21</v>
-      </c>
-      <c r="E47" t="s">
+      <c r="M45" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A48" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="50" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H50" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="I50" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="51" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H51" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="I51" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H52" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I52" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H53" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="I53" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H54" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F47" t="s">
-        <v>67</v>
-      </c>
-      <c r="G47">
-        <v>2024</v>
-      </c>
-      <c r="H47">
+      <c r="I54" s="8">
         <v>3</v>
       </c>
-      <c r="I47">
+    </row>
+    <row r="55" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H55" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I55" s="8">
         <v>2</v>
       </c>
-      <c r="J47">
-        <v>0.25</v>
-      </c>
-      <c r="K47">
-        <f t="shared" si="2"/>
-        <v>2028</v>
-      </c>
-      <c r="L47">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="M47" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H52" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="I52" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H53" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="I53" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H54" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="I54" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H55" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="I55" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H56" s="7" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="I56" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H57" s="7" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="I57" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H58" s="7" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I58" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H59" s="7" t="s">
-        <v>19</v>
+        <v>133</v>
       </c>
       <c r="I59" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H60" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I60" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H61" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I61" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H62" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="I62" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H60" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="I60" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H61" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="I61" s="8">
+    <row r="63" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H63" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="I63" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H62" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="I62" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H63" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="I63" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H64" s="7" t="s">
-        <v>125</v>
+        <v>17</v>
       </c>
       <c r="I64" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H65" s="7" t="s">
-        <v>111</v>
+        <v>12</v>
       </c>
       <c r="I65" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="8:9" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H66" s="7" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="I66" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H67" s="7" t="s">
-        <v>12</v>
+        <v>130</v>
       </c>
       <c r="I67" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="68" spans="8:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H68" s="7" t="s">
-        <v>8</v>
+        <v>139</v>
       </c>
       <c r="I68" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H69" s="7" t="s">
-        <v>130</v>
+        <v>103</v>
       </c>
       <c r="I69" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H70" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="I70" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="71" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H71" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="I71" s="8">
         <v>39</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="E8:E47" xr:uid="{57F1FF48-4396-4FE3-ABD9-234FB66F60F4}"/>
+  <autoFilter ref="E8:E45" xr:uid="{57F1FF48-4396-4FE3-ABD9-234FB66F60F4}"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>

</xml_diff>